<commit_message>
parsing, plotting, and saving survey data
</commit_message>
<xml_diff>
--- a/analysis/scheduler_notes_29Jul2024.xlsx
+++ b/analysis/scheduler_notes_29Jul2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsun\Documents\Code\RTmocapFB\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5484AA5C-74A2-4291-80CE-5CF2E1C2C199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F36D60-3EF0-47CB-B872-C79B2D987297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38265" yWindow="-135" windowWidth="38670" windowHeight="21270" activeTab="5" xr2:uid="{5184CD76-0F71-4C54-9199-95839C9F3B68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{5184CD76-0F71-4C54-9199-95839C9F3B68}"/>
   </bookViews>
   <sheets>
     <sheet name="April" sheetId="1" r:id="rId1"/>
@@ -1367,15 +1367,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1387,6 +1378,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1732,17 +1732,17 @@
       <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="3" customWidth="1"/>
-    <col min="3" max="14" width="5.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="3" customWidth="1"/>
+    <col min="3" max="14" width="5.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="1"/>
     <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="116"/>
       <c r="B1" s="117"/>
       <c r="C1" s="114" t="s">
@@ -1758,7 +1758,7 @@
       <c r="K1" s="114"/>
       <c r="L1" s="115"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="118"/>
       <c r="B2" s="119"/>
       <c r="C2" s="12" t="s">
@@ -1798,7 +1798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="120" t="s">
         <v>6</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="120"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -1864,7 +1864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="120"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
@@ -1887,7 +1887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="120"/>
       <c r="B6" s="9">
         <v>0.375</v>
@@ -1910,7 +1910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="120"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
@@ -1932,7 +1932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="120"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
@@ -1948,7 +1948,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="120"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -1964,7 +1964,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="120"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -1980,7 +1980,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="120"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -1996,7 +1996,7 @@
       <c r="K11" s="14"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="120"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -2012,7 +2012,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="120"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -2028,7 +2028,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="120"/>
       <c r="B14" s="9">
         <v>0.54166666666666696</v>
@@ -2044,7 +2044,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="120"/>
       <c r="B15" s="9">
         <v>0.5625</v>
@@ -2060,7 +2060,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="120"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
@@ -2076,7 +2076,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="15"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="120"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
@@ -2092,7 +2092,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="120"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -2108,7 +2108,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="120"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
@@ -2124,7 +2124,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="120"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
@@ -2140,7 +2140,7 @@
       <c r="K20" s="17"/>
       <c r="L20" s="15"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="120"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -2156,7 +2156,7 @@
       <c r="K21" s="17"/>
       <c r="L21" s="18"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="120"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
@@ -2175,7 +2175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="120"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
@@ -2191,7 +2191,7 @@
       <c r="K23" s="14"/>
       <c r="L23" s="15"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="120"/>
       <c r="B24" s="9">
         <v>0.75</v>
@@ -2207,7 +2207,7 @@
       <c r="K24" s="14"/>
       <c r="L24" s="15"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="120"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -2223,7 +2223,7 @@
       <c r="K25" s="14"/>
       <c r="L25" s="15"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="120"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -2239,7 +2239,7 @@
       <c r="K26" s="14"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="121"/>
       <c r="B27" s="19">
         <v>0.812500000000001</v>
@@ -2276,17 +2276,17 @@
       <selection activeCell="AE14" sqref="AE14:AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="35" width="5.5703125" customWidth="1"/>
-    <col min="37" max="37" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="35" width="5.5546875" customWidth="1"/>
+    <col min="37" max="37" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127"/>
-      <c r="B1" s="128"/>
+    <row r="1" spans="1:41" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="124"/>
+      <c r="B1" s="125"/>
       <c r="C1" s="114" t="s">
         <v>8</v>
       </c>
@@ -2321,9 +2321,9 @@
       <c r="AF1" s="114"/>
       <c r="AG1" s="115"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="129"/>
-      <c r="B2" s="130"/>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A2" s="126"/>
+      <c r="B2" s="127"/>
       <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2430,7 +2430,7 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
     </row>
-    <row r="3" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="120" t="s">
         <v>6</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="120"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -2579,7 +2579,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="120"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
@@ -2622,7 +2622,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="120"/>
       <c r="B6" s="9">
         <v>0.375</v>
@@ -2650,7 +2650,7 @@
       <c r="W6" s="36"/>
       <c r="X6" s="34"/>
       <c r="Y6" s="41"/>
-      <c r="Z6" s="126" t="s">
+      <c r="Z6" s="129" t="s">
         <v>32</v>
       </c>
       <c r="AA6" s="49"/>
@@ -2658,10 +2658,10 @@
       <c r="AC6" s="41"/>
       <c r="AD6" s="41"/>
       <c r="AE6" s="34"/>
-      <c r="AF6" s="124" t="s">
+      <c r="AF6" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="AG6" s="125" t="s">
+      <c r="AG6" s="130" t="s">
         <v>40</v>
       </c>
       <c r="AJ6" s="46" t="s">
@@ -2671,7 +2671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="120"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
@@ -2682,7 +2682,7 @@
       <c r="F7" s="49"/>
       <c r="G7" s="53"/>
       <c r="H7" s="43"/>
-      <c r="I7" s="124" t="s">
+      <c r="I7" s="128" t="s">
         <v>26</v>
       </c>
       <c r="J7" s="43"/>
@@ -2701,16 +2701,16 @@
       <c r="W7" s="36"/>
       <c r="X7" s="34"/>
       <c r="Y7" s="41"/>
-      <c r="Z7" s="126"/>
+      <c r="Z7" s="129"/>
       <c r="AA7" s="49"/>
       <c r="AB7" s="41"/>
       <c r="AC7" s="41"/>
-      <c r="AD7" s="126" t="s">
+      <c r="AD7" s="129" t="s">
         <v>35</v>
       </c>
       <c r="AE7" s="34"/>
-      <c r="AF7" s="124"/>
-      <c r="AG7" s="125"/>
+      <c r="AF7" s="128"/>
+      <c r="AG7" s="130"/>
       <c r="AJ7" s="27" t="s">
         <v>20</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="120"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
@@ -2729,8 +2729,8 @@
       <c r="F8" s="49"/>
       <c r="G8" s="53"/>
       <c r="H8" s="43"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="126" t="s">
+      <c r="I8" s="128"/>
+      <c r="J8" s="129" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="31"/>
@@ -2748,14 +2748,14 @@
       <c r="W8" s="36"/>
       <c r="X8" s="34"/>
       <c r="Y8" s="41"/>
-      <c r="Z8" s="126"/>
+      <c r="Z8" s="129"/>
       <c r="AA8" s="49"/>
       <c r="AB8" s="41"/>
       <c r="AC8" s="44"/>
-      <c r="AD8" s="126"/>
+      <c r="AD8" s="129"/>
       <c r="AE8" s="34"/>
       <c r="AF8" s="31"/>
-      <c r="AG8" s="125"/>
+      <c r="AG8" s="130"/>
       <c r="AJ8" s="28" t="s">
         <v>21</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="120"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -2775,7 +2775,7 @@
       <c r="G9" s="53"/>
       <c r="H9" s="17"/>
       <c r="I9" s="43"/>
-      <c r="J9" s="126"/>
+      <c r="J9" s="129"/>
       <c r="K9" s="31"/>
       <c r="L9" s="43"/>
       <c r="M9" s="54"/>
@@ -2795,14 +2795,14 @@
       <c r="AA9" s="49"/>
       <c r="AB9" s="41"/>
       <c r="AC9" s="44"/>
-      <c r="AD9" s="126"/>
+      <c r="AD9" s="129"/>
       <c r="AE9" s="34"/>
-      <c r="AF9" s="124" t="s">
+      <c r="AF9" s="128" t="s">
         <v>45</v>
       </c>
       <c r="AG9" s="15"/>
     </row>
-    <row r="10" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="120"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -2813,10 +2813,10 @@
       <c r="F10" s="49"/>
       <c r="G10" s="53"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="124" t="s">
+      <c r="I10" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="126"/>
+      <c r="J10" s="129"/>
       <c r="K10" s="31"/>
       <c r="L10" s="43"/>
       <c r="M10" s="54"/>
@@ -2838,12 +2838,12 @@
       <c r="AC10" s="41"/>
       <c r="AD10" s="34"/>
       <c r="AE10" s="34"/>
-      <c r="AF10" s="124"/>
-      <c r="AG10" s="125" t="s">
+      <c r="AF10" s="128"/>
+      <c r="AG10" s="130" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="120"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -2854,7 +2854,7 @@
       <c r="F11" s="49"/>
       <c r="G11" s="53"/>
       <c r="H11" s="43"/>
-      <c r="I11" s="124"/>
+      <c r="I11" s="128"/>
       <c r="J11" s="43"/>
       <c r="K11" s="31"/>
       <c r="L11" s="43"/>
@@ -2878,9 +2878,9 @@
       <c r="AD11" s="34"/>
       <c r="AE11" s="34"/>
       <c r="AF11" s="31"/>
-      <c r="AG11" s="125"/>
-    </row>
-    <row r="12" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG11" s="130"/>
+    </row>
+    <row r="12" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="120"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -2907,7 +2907,7 @@
       <c r="V12" s="31"/>
       <c r="W12" s="36"/>
       <c r="X12" s="34"/>
-      <c r="Y12" s="124" t="s">
+      <c r="Y12" s="128" t="s">
         <v>32</v>
       </c>
       <c r="Z12" s="41"/>
@@ -2917,9 +2917,9 @@
       <c r="AD12" s="40"/>
       <c r="AE12" s="34"/>
       <c r="AF12" s="31"/>
-      <c r="AG12" s="125"/>
-    </row>
-    <row r="13" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG12" s="130"/>
+    </row>
+    <row r="13" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="120"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -2946,7 +2946,7 @@
       <c r="V13" s="31"/>
       <c r="W13" s="36"/>
       <c r="X13" s="34"/>
-      <c r="Y13" s="124"/>
+      <c r="Y13" s="128"/>
       <c r="Z13" s="41"/>
       <c r="AA13" s="49"/>
       <c r="AB13" s="41"/>
@@ -2956,7 +2956,7 @@
       <c r="AF13" s="31"/>
       <c r="AG13" s="15"/>
     </row>
-    <row r="14" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="120"/>
       <c r="B14" s="9">
         <v>0.54166666666666663</v>
@@ -2983,25 +2983,25 @@
       <c r="V14" s="31"/>
       <c r="W14" s="36"/>
       <c r="X14" s="34"/>
-      <c r="Y14" s="124" t="s">
+      <c r="Y14" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="Z14" s="126" t="s">
+      <c r="Z14" s="129" t="s">
         <v>33</v>
       </c>
       <c r="AA14" s="49"/>
       <c r="AB14" s="41"/>
       <c r="AC14" s="41"/>
-      <c r="AD14" s="126" t="s">
+      <c r="AD14" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="AE14" s="126" t="s">
+      <c r="AE14" s="129" t="s">
         <v>39</v>
       </c>
       <c r="AF14" s="31"/>
       <c r="AG14" s="15"/>
     </row>
-    <row r="15" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="120"/>
       <c r="B15" s="9">
         <v>0.5625</v>
@@ -3028,17 +3028,17 @@
       <c r="V15" s="31"/>
       <c r="W15" s="36"/>
       <c r="X15" s="34"/>
-      <c r="Y15" s="124"/>
-      <c r="Z15" s="126"/>
+      <c r="Y15" s="128"/>
+      <c r="Z15" s="129"/>
       <c r="AA15" s="49"/>
       <c r="AB15" s="41"/>
       <c r="AC15" s="41"/>
-      <c r="AD15" s="126"/>
-      <c r="AE15" s="126"/>
+      <c r="AD15" s="129"/>
+      <c r="AE15" s="129"/>
       <c r="AF15" s="31"/>
       <c r="AG15" s="15"/>
     </row>
-    <row r="16" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="120"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
@@ -3066,18 +3066,18 @@
       <c r="W16" s="36"/>
       <c r="X16" s="34"/>
       <c r="Y16" s="41"/>
-      <c r="Z16" s="126"/>
+      <c r="Z16" s="129"/>
       <c r="AA16" s="49"/>
       <c r="AB16" s="41"/>
       <c r="AC16" s="36"/>
-      <c r="AD16" s="126"/>
-      <c r="AE16" s="126"/>
-      <c r="AF16" s="126" t="s">
+      <c r="AD16" s="129"/>
+      <c r="AE16" s="129"/>
+      <c r="AF16" s="129" t="s">
         <v>41</v>
       </c>
       <c r="AG16" s="70"/>
     </row>
-    <row r="17" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="120"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
@@ -3089,7 +3089,7 @@
       <c r="G17" s="53"/>
       <c r="H17" s="16"/>
       <c r="I17" s="43"/>
-      <c r="J17" s="126" t="s">
+      <c r="J17" s="129" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="31"/>
@@ -3113,10 +3113,10 @@
       <c r="AC17" s="36"/>
       <c r="AD17" s="41"/>
       <c r="AE17" s="34"/>
-      <c r="AF17" s="126"/>
+      <c r="AF17" s="129"/>
       <c r="AG17" s="70"/>
     </row>
-    <row r="18" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="120"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -3128,7 +3128,7 @@
       <c r="G18" s="53"/>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
-      <c r="J18" s="126"/>
+      <c r="J18" s="129"/>
       <c r="K18" s="31"/>
       <c r="L18" s="43"/>
       <c r="M18" s="54"/>
@@ -3148,14 +3148,14 @@
       <c r="AA18" s="49"/>
       <c r="AB18" s="41"/>
       <c r="AC18" s="36"/>
-      <c r="AD18" s="124" t="s">
+      <c r="AD18" s="128" t="s">
         <v>39</v>
       </c>
       <c r="AE18" s="34"/>
-      <c r="AF18" s="126"/>
+      <c r="AF18" s="129"/>
       <c r="AG18" s="17"/>
     </row>
-    <row r="19" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
@@ -3167,7 +3167,7 @@
       <c r="G19" s="53"/>
       <c r="H19" s="43"/>
       <c r="I19" s="43"/>
-      <c r="J19" s="126"/>
+      <c r="J19" s="129"/>
       <c r="K19" s="31"/>
       <c r="L19" s="43"/>
       <c r="M19" s="54"/>
@@ -3187,14 +3187,14 @@
       <c r="AA19" s="49"/>
       <c r="AB19" s="41"/>
       <c r="AC19" s="41"/>
-      <c r="AD19" s="124"/>
-      <c r="AE19" s="124" t="s">
+      <c r="AD19" s="128"/>
+      <c r="AE19" s="128" t="s">
         <v>41</v>
       </c>
       <c r="AF19" s="31"/>
       <c r="AG19" s="17"/>
     </row>
-    <row r="20" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="120"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
@@ -3225,15 +3225,15 @@
       <c r="Z20" s="41"/>
       <c r="AA20" s="49"/>
       <c r="AB20" s="41"/>
-      <c r="AC20" s="124" t="s">
+      <c r="AC20" s="128" t="s">
         <v>34</v>
       </c>
       <c r="AD20" s="41"/>
-      <c r="AE20" s="124"/>
+      <c r="AE20" s="128"/>
       <c r="AF20" s="31"/>
       <c r="AG20" s="17"/>
     </row>
-    <row r="21" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="120"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -3264,13 +3264,13 @@
       <c r="Z21" s="41"/>
       <c r="AA21" s="49"/>
       <c r="AB21" s="41"/>
-      <c r="AC21" s="124"/>
+      <c r="AC21" s="128"/>
       <c r="AD21" s="41"/>
       <c r="AE21" s="34"/>
       <c r="AF21" s="31"/>
       <c r="AG21" s="15"/>
     </row>
-    <row r="22" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="120"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
@@ -3301,7 +3301,7 @@
       <c r="Z22" s="41"/>
       <c r="AA22" s="49"/>
       <c r="AB22" s="41"/>
-      <c r="AC22" s="124" t="s">
+      <c r="AC22" s="128" t="s">
         <v>35</v>
       </c>
       <c r="AD22" s="41"/>
@@ -3309,7 +3309,7 @@
       <c r="AF22" s="31"/>
       <c r="AG22" s="15"/>
     </row>
-    <row r="23" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="120"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
@@ -3340,13 +3340,13 @@
       <c r="Z23" s="41"/>
       <c r="AA23" s="49"/>
       <c r="AB23" s="41"/>
-      <c r="AC23" s="124"/>
+      <c r="AC23" s="128"/>
       <c r="AD23" s="41"/>
       <c r="AE23" s="34"/>
       <c r="AF23" s="31"/>
       <c r="AG23" s="15"/>
     </row>
-    <row r="24" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="120"/>
       <c r="B24" s="9">
         <v>0.75</v>
@@ -3383,7 +3383,7 @@
       <c r="AF24" s="31"/>
       <c r="AG24" s="15"/>
     </row>
-    <row r="25" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="120"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -3420,7 +3420,7 @@
       <c r="AF25" s="31"/>
       <c r="AG25" s="15"/>
     </row>
-    <row r="26" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="120"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -3457,7 +3457,7 @@
       <c r="AF26" s="31"/>
       <c r="AG26" s="15"/>
     </row>
-    <row r="27" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="121"/>
       <c r="B27" s="19">
         <v>0.812500000000001</v>
@@ -3494,7 +3494,7 @@
       <c r="AF27" s="32"/>
       <c r="AG27" s="21"/>
     </row>
-    <row r="28" spans="1:37" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="X28" s="38" t="s">
         <v>28</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="46.8" x14ac:dyDescent="0.3">
       <c r="AJ29" s="38" t="s">
         <v>29</v>
       </c>
@@ -3512,6 +3512,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="AF6:AF7"/>
+    <mergeCell ref="AG6:AG8"/>
+    <mergeCell ref="AD14:AD16"/>
+    <mergeCell ref="AD18:AD19"/>
+    <mergeCell ref="AE14:AE16"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG10:AG12"/>
     <mergeCell ref="C1:AG1"/>
     <mergeCell ref="A3:A27"/>
     <mergeCell ref="A1:B2"/>
@@ -3528,13 +3535,6 @@
     <mergeCell ref="AC20:AC21"/>
     <mergeCell ref="AE19:AE20"/>
     <mergeCell ref="AF16:AF18"/>
-    <mergeCell ref="AF6:AF7"/>
-    <mergeCell ref="AG6:AG8"/>
-    <mergeCell ref="AD14:AD16"/>
-    <mergeCell ref="AD18:AD19"/>
-    <mergeCell ref="AE14:AE16"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG10:AG12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3550,18 +3550,18 @@
       <selection activeCell="AJ35" sqref="AJ35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="10"/>
-    <col min="2" max="34" width="5.85546875" style="2" customWidth="1"/>
-    <col min="35" max="35" width="8.85546875" style="2"/>
-    <col min="36" max="36" width="44.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="10"/>
+    <col min="2" max="34" width="5.88671875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="8.88671875" style="2"/>
+    <col min="36" max="36" width="44.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127"/>
-      <c r="B1" s="128"/>
+    <row r="1" spans="1:36" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="124"/>
+      <c r="B1" s="125"/>
       <c r="C1" s="114" t="s">
         <v>11</v>
       </c>
@@ -3595,9 +3595,9 @@
       <c r="AE1" s="114"/>
       <c r="AF1" s="115"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="129"/>
-      <c r="B2" s="130"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A2" s="126"/>
+      <c r="B2" s="127"/>
       <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="120" t="s">
         <v>6</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="120"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -3829,7 +3829,7 @@
       <c r="AA4" s="75"/>
       <c r="AB4" s="75"/>
       <c r="AC4" s="75"/>
-      <c r="AD4" s="126" t="s">
+      <c r="AD4" s="129" t="s">
         <v>65</v>
       </c>
       <c r="AE4" s="71"/>
@@ -3841,17 +3841,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="120"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="73"/>
-      <c r="E5" s="124" t="s">
+      <c r="E5" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="126" t="s">
+      <c r="F5" s="129" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="75"/>
@@ -3877,7 +3877,7 @@
       <c r="AA5" s="75"/>
       <c r="AB5" s="75"/>
       <c r="AC5" s="75"/>
-      <c r="AD5" s="126"/>
+      <c r="AD5" s="129"/>
       <c r="AE5" s="71"/>
       <c r="AF5" s="84"/>
       <c r="AI5" s="62" t="s">
@@ -3887,57 +3887,57 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="120"/>
       <c r="B6" s="9">
         <v>0.375</v>
       </c>
       <c r="C6" s="71"/>
       <c r="D6" s="73"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="126"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="129"/>
       <c r="G6" s="75"/>
       <c r="H6" s="75"/>
-      <c r="I6" s="126" t="s">
+      <c r="I6" s="129" t="s">
         <v>48</v>
       </c>
       <c r="J6" s="71"/>
       <c r="K6" s="73"/>
-      <c r="L6" s="124" t="s">
+      <c r="L6" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="124" t="s">
+      <c r="M6" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="126" t="s">
+      <c r="N6" s="129" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="75"/>
       <c r="P6" s="71"/>
       <c r="Q6" s="71"/>
       <c r="R6" s="73"/>
-      <c r="S6" s="124" t="s">
+      <c r="S6" s="128" t="s">
         <v>53</v>
       </c>
-      <c r="T6" s="126" t="s">
+      <c r="T6" s="129" t="s">
         <v>53</v>
       </c>
       <c r="U6" s="75"/>
-      <c r="V6" s="124" t="s">
+      <c r="V6" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="W6" s="126" t="s">
+      <c r="W6" s="129" t="s">
         <v>59</v>
       </c>
       <c r="X6" s="71"/>
       <c r="Y6" s="57"/>
-      <c r="Z6" s="124" t="s">
+      <c r="Z6" s="128" t="s">
         <v>61</v>
       </c>
       <c r="AA6" s="75"/>
       <c r="AB6" s="75"/>
       <c r="AC6" s="75"/>
-      <c r="AD6" s="126"/>
+      <c r="AD6" s="129"/>
       <c r="AE6" s="71"/>
       <c r="AF6" s="84"/>
       <c r="AI6" s="63" t="s">
@@ -3947,7 +3947,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="120"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
@@ -3955,31 +3955,31 @@
       <c r="C7" s="71"/>
       <c r="D7" s="73"/>
       <c r="E7" s="75"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="124" t="s">
+      <c r="F7" s="129"/>
+      <c r="G7" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="126" t="s">
+      <c r="H7" s="129" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="126"/>
+      <c r="I7" s="129"/>
       <c r="J7" s="71"/>
       <c r="K7" s="73"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="124"/>
-      <c r="N7" s="126"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="128"/>
+      <c r="N7" s="129"/>
       <c r="O7" s="75"/>
       <c r="P7" s="71"/>
       <c r="Q7" s="71"/>
       <c r="R7" s="73"/>
-      <c r="S7" s="124"/>
-      <c r="T7" s="126"/>
+      <c r="S7" s="128"/>
+      <c r="T7" s="129"/>
       <c r="U7" s="75"/>
-      <c r="V7" s="124"/>
-      <c r="W7" s="126"/>
+      <c r="V7" s="128"/>
+      <c r="W7" s="129"/>
       <c r="X7" s="71"/>
       <c r="Y7" s="57"/>
-      <c r="Z7" s="124"/>
+      <c r="Z7" s="128"/>
       <c r="AA7" s="75"/>
       <c r="AB7" s="75"/>
       <c r="AC7" s="75"/>
@@ -3993,7 +3993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="120"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
@@ -4002,37 +4002,37 @@
       <c r="D8" s="73"/>
       <c r="E8" s="75"/>
       <c r="F8" s="75"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
       <c r="J8" s="71"/>
       <c r="K8" s="73"/>
       <c r="L8" s="71"/>
       <c r="M8" s="75"/>
-      <c r="N8" s="126"/>
-      <c r="O8" s="124" t="s">
+      <c r="N8" s="129"/>
+      <c r="O8" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="126" t="s">
+      <c r="P8" s="129" t="s">
         <v>49</v>
       </c>
       <c r="Q8" s="71"/>
       <c r="R8" s="73"/>
       <c r="S8" s="75"/>
-      <c r="T8" s="126"/>
-      <c r="U8" s="126" t="s">
+      <c r="T8" s="129"/>
+      <c r="U8" s="129" t="s">
         <v>55</v>
       </c>
       <c r="V8" s="75"/>
-      <c r="W8" s="126"/>
+      <c r="W8" s="129"/>
       <c r="X8" s="71"/>
       <c r="Y8" s="57"/>
       <c r="Z8" s="75"/>
       <c r="AA8" s="17"/>
-      <c r="AB8" s="124" t="s">
+      <c r="AB8" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="AC8" s="126" t="s">
+      <c r="AC8" s="129" t="s">
         <v>56</v>
       </c>
       <c r="AD8" s="71"/>
@@ -4045,7 +4045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="120"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -4055,25 +4055,25 @@
       <c r="E9" s="69"/>
       <c r="F9" s="75"/>
       <c r="G9" s="75"/>
-      <c r="H9" s="126"/>
+      <c r="H9" s="129"/>
       <c r="I9" s="71"/>
       <c r="J9" s="71"/>
       <c r="K9" s="73"/>
       <c r="L9" s="71"/>
-      <c r="M9" s="124" t="s">
+      <c r="M9" s="128" t="s">
         <v>52</v>
       </c>
       <c r="N9" s="75"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="126"/>
+      <c r="O9" s="128"/>
+      <c r="P9" s="129"/>
       <c r="Q9" s="71"/>
       <c r="R9" s="73"/>
-      <c r="S9" s="124" t="s">
+      <c r="S9" s="128" t="s">
         <v>54</v>
       </c>
       <c r="T9" s="75"/>
-      <c r="U9" s="126"/>
-      <c r="V9" s="126" t="s">
+      <c r="U9" s="129"/>
+      <c r="V9" s="129" t="s">
         <v>60</v>
       </c>
       <c r="W9" s="71"/>
@@ -4081,8 +4081,8 @@
       <c r="Y9" s="57"/>
       <c r="Z9" s="75"/>
       <c r="AA9" s="17"/>
-      <c r="AB9" s="124"/>
-      <c r="AC9" s="126"/>
+      <c r="AB9" s="128"/>
+      <c r="AC9" s="129"/>
       <c r="AD9" s="71"/>
       <c r="AE9" s="71"/>
       <c r="AF9" s="84"/>
@@ -4093,7 +4093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="120"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -4108,32 +4108,32 @@
       <c r="J10" s="71"/>
       <c r="K10" s="73"/>
       <c r="L10" s="71"/>
-      <c r="M10" s="124"/>
-      <c r="N10" s="126" t="s">
+      <c r="M10" s="128"/>
+      <c r="N10" s="129" t="s">
         <v>52</v>
       </c>
       <c r="O10" s="75"/>
-      <c r="P10" s="126"/>
+      <c r="P10" s="129"/>
       <c r="Q10" s="71"/>
       <c r="R10" s="73"/>
-      <c r="S10" s="124"/>
-      <c r="T10" s="126" t="s">
+      <c r="S10" s="128"/>
+      <c r="T10" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="126"/>
-      <c r="V10" s="126"/>
+      <c r="U10" s="129"/>
+      <c r="V10" s="129"/>
       <c r="W10" s="71"/>
       <c r="X10" s="71"/>
       <c r="Y10" s="57"/>
       <c r="Z10" s="75"/>
       <c r="AA10" s="17"/>
       <c r="AB10" s="75"/>
-      <c r="AC10" s="126"/>
+      <c r="AC10" s="129"/>
       <c r="AD10" s="71"/>
       <c r="AE10" s="71"/>
       <c r="AF10" s="84"/>
     </row>
-    <row r="11" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="120"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -4143,25 +4143,25 @@
       <c r="E11" s="69"/>
       <c r="F11" s="75"/>
       <c r="G11" s="75"/>
-      <c r="H11" s="124" t="s">
+      <c r="H11" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="126" t="s">
+      <c r="I11" s="129" t="s">
         <v>47</v>
       </c>
       <c r="J11" s="71"/>
       <c r="K11" s="73"/>
       <c r="L11" s="71"/>
       <c r="M11" s="75"/>
-      <c r="N11" s="126"/>
+      <c r="N11" s="129"/>
       <c r="O11" s="75"/>
       <c r="P11" s="71"/>
       <c r="Q11" s="71"/>
       <c r="R11" s="73"/>
       <c r="S11" s="75"/>
-      <c r="T11" s="126"/>
+      <c r="T11" s="129"/>
       <c r="U11" s="75"/>
-      <c r="V11" s="126"/>
+      <c r="V11" s="129"/>
       <c r="W11" s="71"/>
       <c r="X11" s="71"/>
       <c r="Y11" s="57"/>
@@ -4173,7 +4173,7 @@
       <c r="AE11" s="71"/>
       <c r="AF11" s="84"/>
     </row>
-    <row r="12" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="120"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -4183,21 +4183,21 @@
       <c r="E12" s="69"/>
       <c r="F12" s="75"/>
       <c r="G12" s="75"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="126"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="129"/>
       <c r="J12" s="71"/>
       <c r="K12" s="73"/>
       <c r="L12" s="71"/>
       <c r="M12" s="75"/>
-      <c r="N12" s="126"/>
+      <c r="N12" s="129"/>
       <c r="O12" s="75"/>
-      <c r="P12" s="126" t="s">
+      <c r="P12" s="129" t="s">
         <v>66</v>
       </c>
       <c r="Q12" s="71"/>
       <c r="R12" s="73"/>
       <c r="S12" s="75"/>
-      <c r="T12" s="126"/>
+      <c r="T12" s="129"/>
       <c r="U12" s="75"/>
       <c r="V12" s="75"/>
       <c r="W12" s="71"/>
@@ -4211,7 +4211,7 @@
       <c r="AE12" s="71"/>
       <c r="AF12" s="84"/>
     </row>
-    <row r="13" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="120"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -4222,19 +4222,19 @@
       <c r="F13" s="75"/>
       <c r="G13" s="75"/>
       <c r="H13" s="75"/>
-      <c r="I13" s="126"/>
+      <c r="I13" s="129"/>
       <c r="J13" s="71"/>
       <c r="K13" s="73"/>
       <c r="L13" s="71"/>
       <c r="M13" s="75"/>
       <c r="N13" s="75"/>
       <c r="O13" s="75"/>
-      <c r="P13" s="126"/>
+      <c r="P13" s="129"/>
       <c r="Q13" s="71"/>
       <c r="R13" s="73"/>
       <c r="S13" s="75"/>
       <c r="T13" s="75"/>
-      <c r="U13" s="124" t="s">
+      <c r="U13" s="128" t="s">
         <v>60</v>
       </c>
       <c r="V13" s="75"/>
@@ -4249,7 +4249,7 @@
       <c r="AE13" s="71"/>
       <c r="AF13" s="84"/>
     </row>
-    <row r="14" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="120"/>
       <c r="B14" s="9">
         <v>0.54166666666666696</v>
@@ -4257,32 +4257,32 @@
       <c r="C14" s="71"/>
       <c r="D14" s="73"/>
       <c r="E14" s="75"/>
-      <c r="F14" s="126" t="s">
+      <c r="F14" s="129" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="75"/>
-      <c r="H14" s="124" t="s">
+      <c r="H14" s="128" t="s">
         <v>48</v>
       </c>
       <c r="I14" s="71"/>
       <c r="J14" s="71"/>
       <c r="K14" s="73"/>
       <c r="L14" s="71"/>
-      <c r="M14" s="126" t="s">
+      <c r="M14" s="129" t="s">
         <v>51</v>
       </c>
-      <c r="N14" s="124" t="s">
+      <c r="N14" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="126" t="s">
+      <c r="O14" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="P14" s="126"/>
+      <c r="P14" s="129"/>
       <c r="Q14" s="71"/>
       <c r="R14" s="73"/>
       <c r="S14" s="75"/>
       <c r="T14" s="75"/>
-      <c r="U14" s="124"/>
+      <c r="U14" s="128"/>
       <c r="V14" s="75"/>
       <c r="W14" s="71"/>
       <c r="X14" s="71"/>
@@ -4295,26 +4295,26 @@
       <c r="AE14" s="71"/>
       <c r="AF14" s="84"/>
     </row>
-    <row r="15" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="120"/>
       <c r="B15" s="9">
         <v>0.5625</v>
       </c>
       <c r="C15" s="71"/>
       <c r="D15" s="73"/>
-      <c r="E15" s="124" t="s">
+      <c r="E15" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="126"/>
+      <c r="F15" s="129"/>
       <c r="G15" s="75"/>
-      <c r="H15" s="124"/>
+      <c r="H15" s="128"/>
       <c r="I15" s="71"/>
       <c r="J15" s="71"/>
       <c r="K15" s="73"/>
       <c r="L15" s="71"/>
-      <c r="M15" s="126"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="126"/>
+      <c r="M15" s="129"/>
+      <c r="N15" s="128"/>
+      <c r="O15" s="129"/>
       <c r="P15" s="71"/>
       <c r="Q15" s="71"/>
       <c r="R15" s="73"/>
@@ -4326,7 +4326,7 @@
       <c r="X15" s="71"/>
       <c r="Y15" s="57"/>
       <c r="Z15" s="75"/>
-      <c r="AA15" s="126" t="s">
+      <c r="AA15" s="129" t="s">
         <v>57</v>
       </c>
       <c r="AB15" s="75"/>
@@ -4335,43 +4335,43 @@
       <c r="AE15" s="71"/>
       <c r="AF15" s="84"/>
     </row>
-    <row r="16" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="120"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
       </c>
       <c r="C16" s="71"/>
       <c r="D16" s="73"/>
-      <c r="E16" s="124"/>
-      <c r="F16" s="126"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="129"/>
       <c r="G16" s="75"/>
       <c r="H16" s="75"/>
       <c r="I16" s="71"/>
       <c r="J16" s="71"/>
       <c r="K16" s="73"/>
       <c r="L16" s="71"/>
-      <c r="M16" s="126"/>
+      <c r="M16" s="129"/>
       <c r="N16" s="75"/>
-      <c r="O16" s="126"/>
+      <c r="O16" s="129"/>
       <c r="P16" s="71"/>
       <c r="Q16" s="71"/>
       <c r="R16" s="73"/>
       <c r="S16" s="33"/>
-      <c r="T16" s="124" t="s">
+      <c r="T16" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="U16" s="124" t="s">
+      <c r="U16" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="V16" s="126" t="s">
+      <c r="V16" s="129" t="s">
         <v>58</v>
       </c>
       <c r="W16" s="71"/>
       <c r="X16" s="71"/>
       <c r="Y16" s="57"/>
       <c r="Z16" s="75"/>
-      <c r="AA16" s="126"/>
-      <c r="AB16" s="124" t="s">
+      <c r="AA16" s="129"/>
+      <c r="AB16" s="128" t="s">
         <v>62</v>
       </c>
       <c r="AC16" s="75"/>
@@ -4379,7 +4379,7 @@
       <c r="AE16" s="71"/>
       <c r="AF16" s="84"/>
     </row>
-    <row r="17" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="120"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
@@ -4401,23 +4401,23 @@
       <c r="Q17" s="71"/>
       <c r="R17" s="73"/>
       <c r="S17" s="33"/>
-      <c r="T17" s="124"/>
-      <c r="U17" s="124"/>
-      <c r="V17" s="126"/>
+      <c r="T17" s="128"/>
+      <c r="U17" s="128"/>
+      <c r="V17" s="129"/>
       <c r="W17" s="71"/>
       <c r="X17" s="71"/>
       <c r="Y17" s="57"/>
       <c r="Z17" s="75"/>
-      <c r="AA17" s="126"/>
-      <c r="AB17" s="124"/>
-      <c r="AC17" s="126" t="s">
+      <c r="AA17" s="129"/>
+      <c r="AB17" s="128"/>
+      <c r="AC17" s="129" t="s">
         <v>62</v>
       </c>
       <c r="AD17" s="71"/>
       <c r="AE17" s="71"/>
       <c r="AF17" s="84"/>
     </row>
-    <row r="18" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="120"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -4441,21 +4441,21 @@
       <c r="S18" s="75"/>
       <c r="T18" s="75"/>
       <c r="U18" s="75"/>
-      <c r="V18" s="126"/>
+      <c r="V18" s="129"/>
       <c r="W18" s="71"/>
       <c r="X18" s="71"/>
       <c r="Y18" s="57"/>
-      <c r="Z18" s="124" t="s">
+      <c r="Z18" s="128" t="s">
         <v>57</v>
       </c>
       <c r="AA18" s="75"/>
       <c r="AB18" s="75"/>
-      <c r="AC18" s="126"/>
+      <c r="AC18" s="129"/>
       <c r="AD18" s="71"/>
       <c r="AE18" s="71"/>
       <c r="AF18" s="84"/>
     </row>
-    <row r="19" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
@@ -4483,15 +4483,15 @@
       <c r="W19" s="71"/>
       <c r="X19" s="71"/>
       <c r="Y19" s="57"/>
-      <c r="Z19" s="124"/>
+      <c r="Z19" s="128"/>
       <c r="AA19" s="75"/>
       <c r="AB19" s="75"/>
-      <c r="AC19" s="126"/>
+      <c r="AC19" s="129"/>
       <c r="AD19" s="71"/>
       <c r="AE19" s="71"/>
       <c r="AF19" s="84"/>
     </row>
-    <row r="20" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="120"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
@@ -4520,7 +4520,7 @@
       <c r="X20" s="71"/>
       <c r="Y20" s="57"/>
       <c r="Z20" s="75"/>
-      <c r="AA20" s="126" t="s">
+      <c r="AA20" s="129" t="s">
         <v>61</v>
       </c>
       <c r="AB20" s="75"/>
@@ -4529,7 +4529,7 @@
       <c r="AE20" s="71"/>
       <c r="AF20" s="84"/>
     </row>
-    <row r="21" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="120"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -4558,16 +4558,16 @@
       <c r="X21" s="71"/>
       <c r="Y21" s="57"/>
       <c r="Z21" s="75"/>
-      <c r="AA21" s="126"/>
+      <c r="AA21" s="129"/>
       <c r="AB21" s="75"/>
-      <c r="AC21" s="124" t="s">
+      <c r="AC21" s="128" t="s">
         <v>65</v>
       </c>
       <c r="AD21" s="71"/>
       <c r="AE21" s="71"/>
       <c r="AF21" s="84"/>
     </row>
-    <row r="22" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="120"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
@@ -4584,7 +4584,7 @@
       <c r="L22" s="17"/>
       <c r="M22" s="75"/>
       <c r="N22" s="75"/>
-      <c r="O22" s="124" t="s">
+      <c r="O22" s="128" t="s">
         <v>66</v>
       </c>
       <c r="P22" s="17"/>
@@ -4598,14 +4598,14 @@
       <c r="X22" s="71"/>
       <c r="Y22" s="57"/>
       <c r="Z22" s="75"/>
-      <c r="AA22" s="126"/>
+      <c r="AA22" s="129"/>
       <c r="AB22" s="75"/>
-      <c r="AC22" s="124"/>
+      <c r="AC22" s="128"/>
       <c r="AD22" s="71"/>
       <c r="AE22" s="71"/>
       <c r="AF22" s="84"/>
     </row>
-    <row r="23" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="120"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
@@ -4622,7 +4622,7 @@
       <c r="L23" s="71"/>
       <c r="M23" s="75"/>
       <c r="N23" s="71"/>
-      <c r="O23" s="124"/>
+      <c r="O23" s="128"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="71"/>
       <c r="R23" s="73"/>
@@ -4641,7 +4641,7 @@
       <c r="AE23" s="71"/>
       <c r="AF23" s="84"/>
     </row>
-    <row r="24" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="120"/>
       <c r="B24" s="9">
         <v>0.75</v>
@@ -4677,7 +4677,7 @@
       <c r="AE24" s="71"/>
       <c r="AF24" s="84"/>
     </row>
-    <row r="25" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="120"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -4713,7 +4713,7 @@
       <c r="AE25" s="71"/>
       <c r="AF25" s="84"/>
     </row>
-    <row r="26" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="120"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -4749,7 +4749,7 @@
       <c r="AE26" s="71"/>
       <c r="AF26" s="84"/>
     </row>
-    <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="121"/>
       <c r="B27" s="19">
         <v>0.812500000000001</v>
@@ -4787,6 +4787,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="U8:U10"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="AC17:AC19"/>
+    <mergeCell ref="AC21:AC22"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T10:T12"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="AC8:AC10"/>
+    <mergeCell ref="Z18:Z19"/>
+    <mergeCell ref="AA15:AA17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="V16:V18"/>
+    <mergeCell ref="AA20:AA22"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W8"/>
     <mergeCell ref="AD4:AD6"/>
     <mergeCell ref="O22:O23"/>
     <mergeCell ref="P12:P14"/>
@@ -4803,37 +4834,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="I6:I8"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="AC17:AC19"/>
-    <mergeCell ref="AC21:AC22"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T10:T12"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="AC8:AC10"/>
-    <mergeCell ref="Z18:Z19"/>
-    <mergeCell ref="AA15:AA17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="V16:V18"/>
-    <mergeCell ref="AA20:AA22"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="U8:U10"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O16"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4848,18 +4848,18 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="10"/>
-    <col min="2" max="35" width="5.85546875" style="2" customWidth="1"/>
-    <col min="36" max="36" width="8.85546875" style="2"/>
-    <col min="37" max="37" width="44.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="10"/>
+    <col min="2" max="35" width="5.88671875" style="2" customWidth="1"/>
+    <col min="36" max="36" width="8.88671875" style="2"/>
+    <col min="37" max="37" width="44.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127"/>
-      <c r="B1" s="128"/>
+    <row r="1" spans="1:37" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="124"/>
+      <c r="B1" s="125"/>
       <c r="C1" s="114" t="s">
         <v>93</v>
       </c>
@@ -4894,9 +4894,9 @@
       <c r="AF1" s="114"/>
       <c r="AG1" s="115"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="129"/>
-      <c r="B2" s="130"/>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A2" s="126"/>
+      <c r="B2" s="127"/>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="120" t="s">
         <v>6</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="120"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -5145,7 +5145,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="120"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
@@ -5188,13 +5188,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="120"/>
       <c r="B6" s="9">
         <v>0.375</v>
       </c>
       <c r="C6" s="71"/>
-      <c r="D6" s="126" t="s">
+      <c r="D6" s="129" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="68"/>
@@ -5233,13 +5233,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="120"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
       </c>
       <c r="C7" s="71"/>
-      <c r="D7" s="126"/>
+      <c r="D7" s="129"/>
       <c r="E7" s="68"/>
       <c r="F7" s="68"/>
       <c r="G7" s="68"/>
@@ -5276,18 +5276,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="120"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
       </c>
       <c r="C8" s="71"/>
-      <c r="D8" s="126"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="68"/>
-      <c r="F8" s="124" t="s">
+      <c r="F8" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="126" t="s">
+      <c r="G8" s="129" t="s">
         <v>67</v>
       </c>
       <c r="H8" s="68"/>
@@ -5317,7 +5317,7 @@
       <c r="AF8" s="71"/>
       <c r="AG8" s="15"/>
     </row>
-    <row r="9" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="120"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -5325,8 +5325,8 @@
       <c r="C9" s="71"/>
       <c r="D9" s="71"/>
       <c r="E9" s="68"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="126"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="129"/>
       <c r="H9" s="68"/>
       <c r="I9" s="73"/>
       <c r="J9" s="71"/>
@@ -5354,7 +5354,7 @@
       <c r="AF9" s="71"/>
       <c r="AG9" s="15"/>
     </row>
-    <row r="10" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="120"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -5363,7 +5363,7 @@
       <c r="D10" s="71"/>
       <c r="E10" s="68"/>
       <c r="F10" s="75"/>
-      <c r="G10" s="126"/>
+      <c r="G10" s="129"/>
       <c r="H10" s="68"/>
       <c r="I10" s="73"/>
       <c r="J10" s="71"/>
@@ -5391,7 +5391,7 @@
       <c r="AF10" s="71"/>
       <c r="AG10" s="15"/>
     </row>
-    <row r="11" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="120"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -5428,7 +5428,7 @@
       <c r="AF11" s="71"/>
       <c r="AG11" s="15"/>
     </row>
-    <row r="12" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="120"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -5465,7 +5465,7 @@
       <c r="AF12" s="71"/>
       <c r="AG12" s="15"/>
     </row>
-    <row r="13" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="120"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -5502,7 +5502,7 @@
       <c r="AF13" s="71"/>
       <c r="AG13" s="15"/>
     </row>
-    <row r="14" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="120"/>
       <c r="B14" s="9">
         <v>0.54166666666666696</v>
@@ -5539,16 +5539,16 @@
       <c r="AF14" s="71"/>
       <c r="AG14" s="15"/>
     </row>
-    <row r="15" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="120"/>
       <c r="B15" s="9">
         <v>0.5625</v>
       </c>
       <c r="C15" s="36"/>
-      <c r="D15" s="124" t="s">
+      <c r="D15" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="126" t="s">
+      <c r="E15" s="129" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="68"/>
@@ -5580,14 +5580,14 @@
       <c r="AF15" s="71"/>
       <c r="AG15" s="15"/>
     </row>
-    <row r="16" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="120"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
       </c>
       <c r="C16" s="36"/>
-      <c r="D16" s="124"/>
-      <c r="E16" s="126"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="68"/>
       <c r="G16" s="68"/>
       <c r="H16" s="68"/>
@@ -5617,14 +5617,14 @@
       <c r="AF16" s="71"/>
       <c r="AG16" s="15"/>
     </row>
-    <row r="17" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="120"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="71"/>
-      <c r="E17" s="126"/>
+      <c r="E17" s="129"/>
       <c r="F17" s="68"/>
       <c r="G17" s="68"/>
       <c r="H17" s="68"/>
@@ -5654,7 +5654,7 @@
       <c r="AF17" s="71"/>
       <c r="AG17" s="15"/>
     </row>
-    <row r="18" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="120"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -5691,12 +5691,12 @@
       <c r="AF18" s="71"/>
       <c r="AG18" s="15"/>
     </row>
-    <row r="19" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
       </c>
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="128" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="71"/>
@@ -5730,12 +5730,12 @@
       <c r="AF19" s="71"/>
       <c r="AG19" s="15"/>
     </row>
-    <row r="20" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="120"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C20" s="124"/>
+      <c r="C20" s="128"/>
       <c r="D20" s="71"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
@@ -5767,7 +5767,7 @@
       <c r="AF20" s="71"/>
       <c r="AG20" s="15"/>
     </row>
-    <row r="21" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="120"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -5804,15 +5804,15 @@
       <c r="AF21" s="71"/>
       <c r="AG21" s="15"/>
     </row>
-    <row r="22" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="120"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C22" s="124" t="s">
+      <c r="C22" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="126" t="s">
+      <c r="D22" s="129" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="17"/>
@@ -5845,13 +5845,13 @@
       <c r="AF22" s="71"/>
       <c r="AG22" s="15"/>
     </row>
-    <row r="23" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="120"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
       </c>
-      <c r="C23" s="124"/>
-      <c r="D23" s="126"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="129"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -5882,13 +5882,13 @@
       <c r="AF23" s="71"/>
       <c r="AG23" s="15"/>
     </row>
-    <row r="24" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="120"/>
       <c r="B24" s="9">
         <v>0.75</v>
       </c>
       <c r="C24" s="71"/>
-      <c r="D24" s="126"/>
+      <c r="D24" s="129"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -5919,7 +5919,7 @@
       <c r="AF24" s="71"/>
       <c r="AG24" s="15"/>
     </row>
-    <row r="25" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="120"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -5956,7 +5956,7 @@
       <c r="AF25" s="71"/>
       <c r="AG25" s="15"/>
     </row>
-    <row r="26" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="120"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -5993,7 +5993,7 @@
       <c r="AF26" s="71"/>
       <c r="AG26" s="15"/>
     </row>
-    <row r="27" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="121"/>
       <c r="B27" s="19">
         <v>0.812500000000001</v>
@@ -6053,34 +6053,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED77502B-B61F-4A2A-AA93-5E2021079CF0}">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="96" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="48.28515625" style="106" customWidth="1"/>
-    <col min="10" max="10" width="185.85546875" style="106" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" style="107" customWidth="1"/>
-    <col min="13" max="15" width="12.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="8.85546875" style="2"/>
-    <col min="21" max="21" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="96" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="48.33203125" style="106" customWidth="1"/>
+    <col min="10" max="10" width="185.88671875" style="106" customWidth="1"/>
+    <col min="11" max="12" width="10.6640625" style="107" customWidth="1"/>
+    <col min="13" max="15" width="12.109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="8.88671875" style="2"/>
+    <col min="21" max="21" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="89" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="89" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="89" t="s">
         <v>36</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -6361,7 +6361,7 @@
       <c r="V6" s="132"/>
       <c r="W6" s="133"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>81.099999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="81" t="s">
         <v>47</v>
       </c>
@@ -6815,7 +6815,7 @@
       <c r="W15" s="132"/>
       <c r="X15" s="133"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="81" t="s">
         <v>48</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>58.6</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>76.900000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>84.2</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>60.2</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="90" t="s">
         <v>63</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -7687,7 +7687,7 @@
       </c>
       <c r="P35" s="107"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>111.1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -7785,29 +7785,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A5247D-4E00-4B4A-AEA2-655372E0F049}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="107" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="107" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="109" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" style="109" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="109" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="110" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="109" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="109" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="109" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="109" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="109" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="109" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="107" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="107" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="109" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.33203125" style="109" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="109" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="110" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" style="109" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="109" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" style="109" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" style="109" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.109375" style="109" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" style="109" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" style="109" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="113" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="113" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
         <v>36</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="107" t="s">
         <v>26</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>0.4861111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="107" t="s">
         <v>27</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>0.61805555555555558</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="107" t="s">
         <v>32</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="107" t="s">
         <v>33</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>0.60069444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="107" t="s">
         <v>34</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>0.59861111111111109</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="107" t="s">
         <v>35</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="107" t="s">
         <v>39</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>0.62152777777777779</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="107" t="s">
         <v>40</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>0.65972222222222221</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="107" t="s">
         <v>41</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>0.4513888888888889</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="107" t="s">
         <v>45</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="107" t="s">
         <v>42</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="107" t="s">
         <v>43</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="107" t="s">
         <v>44</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>0.45624999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="81" t="s">
         <v>47</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>0.53263888888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="81" t="s">
         <v>48</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>0.43402777777777779</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="107" t="s">
         <v>51</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>0.60069444444444442</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="107" t="s">
         <v>50</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="107" t="s">
         <v>52</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="107" t="s">
         <v>46</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="107" t="s">
         <v>49</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="107" t="s">
         <v>66</v>
       </c>
@@ -9105,7 +9105,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="107" t="s">
         <v>53</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="107" t="s">
         <v>54</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>0.51388888888888884</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="107" t="s">
         <v>55</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>0.48819444444444443</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="107" t="s">
         <v>60</v>
       </c>
@@ -9341,7 +9341,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="107" t="s">
         <v>58</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>0.64930555555555558</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="107" t="s">
         <v>59</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="107" t="s">
         <v>61</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>0.73611111111111116</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="107" t="s">
         <v>57</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="107" t="s">
         <v>56</v>
       </c>
@@ -9636,7 +9636,7 @@
         <v>0.49652777777777779</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="107" t="s">
         <v>62</v>
       </c>
@@ -9695,7 +9695,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="107" t="s">
         <v>65</v>
       </c>
@@ -9754,7 +9754,7 @@
         <v>0.39930555555555558</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="107" t="s">
         <v>63</v>
       </c>
@@ -9813,7 +9813,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="107" t="s">
         <v>68</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>0.76041666666666663</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="107" t="s">
         <v>64</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="107" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
the bvp raw data is in weird units..
</commit_message>
<xml_diff>
--- a/analysis/scheduler_notes_29Jul2024.xlsx
+++ b/analysis/scheduler_notes_29Jul2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasu1\Code\RTmocapFB\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsun\Documents\Code\RTmocapFB\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A472345-1CBD-4713-9CB4-870609714026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D279872-C13E-4E53-8E1D-75707310C6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{5184CD76-0F71-4C54-9199-95839C9F3B68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{5184CD76-0F71-4C54-9199-95839C9F3B68}"/>
   </bookViews>
   <sheets>
     <sheet name="April" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Demographics!$A$1:$O$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">EmpaticaData!$A$1:$U$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">EmpaticaData!$A$1:$S$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="150">
   <si>
     <t>Tues</t>
   </si>
@@ -515,12 +515,6 @@
   </si>
   <si>
     <t>Day 2 Date</t>
-  </si>
-  <si>
-    <t>Day 2 Start Epoch</t>
-  </si>
-  <si>
-    <t>Day 2 Retention Start</t>
   </si>
 </sst>
 </file>
@@ -1327,6 +1321,15 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1338,15 +1341,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1390,9 +1384,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1430,7 +1424,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1536,7 +1530,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1678,7 +1672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1692,17 +1686,17 @@
       <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="3" customWidth="1"/>
-    <col min="3" max="14" width="5.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="3" customWidth="1"/>
+    <col min="3" max="14" width="5.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="1"/>
     <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="100"/>
       <c r="B1" s="101"/>
       <c r="C1" s="98" t="s">
@@ -1718,7 +1712,7 @@
       <c r="K1" s="98"/>
       <c r="L1" s="99"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="102"/>
       <c r="B2" s="103"/>
       <c r="C2" s="12" t="s">
@@ -1758,7 +1752,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="104" t="s">
         <v>6</v>
       </c>
@@ -1800,7 +1794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -1824,7 +1818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="104"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
@@ -1847,7 +1841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="104"/>
       <c r="B6" s="9">
         <v>0.375</v>
@@ -1870,7 +1864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
@@ -1892,7 +1886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="104"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
@@ -1908,7 +1902,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="104"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -1924,7 +1918,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="104"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -1940,7 +1934,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="104"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -1956,7 +1950,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="104"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -1972,7 +1966,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="104"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -1988,7 +1982,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="104"/>
       <c r="B14" s="9">
         <v>0.54166666666666696</v>
@@ -2004,7 +1998,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="104"/>
       <c r="B15" s="9">
         <v>0.5625</v>
@@ -2020,7 +2014,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
@@ -2036,7 +2030,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
@@ -2052,7 +2046,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="104"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -2068,7 +2062,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="104"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
@@ -2084,7 +2078,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="104"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
@@ -2100,7 +2094,7 @@
       <c r="K20" s="16"/>
       <c r="L20" s="14"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="104"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -2116,7 +2110,7 @@
       <c r="K21" s="16"/>
       <c r="L21" s="17"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="104"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
@@ -2135,7 +2129,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="104"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
@@ -2151,7 +2145,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="14"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="104"/>
       <c r="B24" s="9">
         <v>0.75</v>
@@ -2167,7 +2161,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="104"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -2183,7 +2177,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="14"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="104"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -2199,7 +2193,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="14"/>
     </row>
-    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="105"/>
       <c r="B27" s="18">
         <v>0.812500000000001</v>
@@ -2236,17 +2230,17 @@
       <selection activeCell="AE14" sqref="AE14:AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="35" width="5.5546875" customWidth="1"/>
-    <col min="37" max="37" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="35" width="5.5703125" customWidth="1"/>
+    <col min="37" max="37" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="108"/>
-      <c r="B1" s="109"/>
+    <row r="1" spans="1:41" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="111"/>
+      <c r="B1" s="112"/>
       <c r="C1" s="98" t="s">
         <v>8</v>
       </c>
@@ -2281,9 +2275,9 @@
       <c r="AF1" s="98"/>
       <c r="AG1" s="99"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A2" s="110"/>
-      <c r="B2" s="111"/>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="113"/>
+      <c r="B2" s="114"/>
       <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2390,7 +2384,7 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
     </row>
-    <row r="3" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="104" t="s">
         <v>6</v>
       </c>
@@ -2496,7 +2490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -2539,7 +2533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="104"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
@@ -2582,7 +2576,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="104"/>
       <c r="B6" s="9">
         <v>0.375</v>
@@ -2610,7 +2604,7 @@
       <c r="W6" s="33"/>
       <c r="X6" s="31"/>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="113" t="s">
+      <c r="Z6" s="110" t="s">
         <v>32</v>
       </c>
       <c r="AA6" s="41"/>
@@ -2618,10 +2612,10 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="31"/>
-      <c r="AF6" s="112" t="s">
+      <c r="AF6" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="AG6" s="114" t="s">
+      <c r="AG6" s="109" t="s">
         <v>40</v>
       </c>
       <c r="AJ6" s="39" t="s">
@@ -2631,7 +2625,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="104"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
@@ -2642,7 +2636,7 @@
       <c r="F7" s="41"/>
       <c r="G7" s="44"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="112" t="s">
+      <c r="I7" s="108" t="s">
         <v>26</v>
       </c>
       <c r="J7" s="2"/>
@@ -2661,16 +2655,16 @@
       <c r="W7" s="33"/>
       <c r="X7" s="31"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="113"/>
+      <c r="Z7" s="110"/>
       <c r="AA7" s="41"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="113" t="s">
+      <c r="AD7" s="110" t="s">
         <v>35</v>
       </c>
       <c r="AE7" s="31"/>
-      <c r="AF7" s="112"/>
-      <c r="AG7" s="114"/>
+      <c r="AF7" s="108"/>
+      <c r="AG7" s="109"/>
       <c r="AJ7" s="24" t="s">
         <v>20</v>
       </c>
@@ -2678,7 +2672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="104"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
@@ -2689,8 +2683,8 @@
       <c r="F8" s="41"/>
       <c r="G8" s="44"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="113" t="s">
+      <c r="I8" s="108"/>
+      <c r="J8" s="110" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="28"/>
@@ -2708,13 +2702,13 @@
       <c r="W8" s="33"/>
       <c r="X8" s="31"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="113"/>
+      <c r="Z8" s="110"/>
       <c r="AA8" s="41"/>
       <c r="AB8" s="2"/>
-      <c r="AD8" s="113"/>
+      <c r="AD8" s="110"/>
       <c r="AE8" s="31"/>
       <c r="AF8" s="28"/>
-      <c r="AG8" s="114"/>
+      <c r="AG8" s="109"/>
       <c r="AJ8" s="25" t="s">
         <v>21</v>
       </c>
@@ -2722,7 +2716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -2734,7 +2728,7 @@
       <c r="G9" s="44"/>
       <c r="H9" s="16"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="113"/>
+      <c r="J9" s="110"/>
       <c r="K9" s="28"/>
       <c r="L9" s="2"/>
       <c r="M9" s="45"/>
@@ -2753,14 +2747,14 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="41"/>
       <c r="AB9" s="2"/>
-      <c r="AD9" s="113"/>
+      <c r="AD9" s="110"/>
       <c r="AE9" s="31"/>
-      <c r="AF9" s="112" t="s">
+      <c r="AF9" s="108" t="s">
         <v>45</v>
       </c>
       <c r="AG9" s="14"/>
     </row>
-    <row r="10" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="104"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -2771,10 +2765,10 @@
       <c r="F10" s="41"/>
       <c r="G10" s="44"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="112" t="s">
+      <c r="I10" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="113"/>
+      <c r="J10" s="110"/>
       <c r="K10" s="28"/>
       <c r="L10" s="2"/>
       <c r="M10" s="45"/>
@@ -2795,12 +2789,12 @@
       <c r="AC10" s="2"/>
       <c r="AD10" s="31"/>
       <c r="AE10" s="31"/>
-      <c r="AF10" s="112"/>
-      <c r="AG10" s="114" t="s">
+      <c r="AF10" s="108"/>
+      <c r="AG10" s="109" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -2811,7 +2805,7 @@
       <c r="F11" s="41"/>
       <c r="G11" s="44"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="112"/>
+      <c r="I11" s="108"/>
       <c r="J11" s="2"/>
       <c r="K11" s="28"/>
       <c r="L11" s="2"/>
@@ -2833,9 +2827,9 @@
       <c r="AD11" s="31"/>
       <c r="AE11" s="31"/>
       <c r="AF11" s="28"/>
-      <c r="AG11" s="114"/>
-    </row>
-    <row r="12" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG11" s="109"/>
+    </row>
+    <row r="12" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -2862,7 +2856,7 @@
       <c r="V12" s="28"/>
       <c r="W12" s="33"/>
       <c r="X12" s="31"/>
-      <c r="Y12" s="112" t="s">
+      <c r="Y12" s="108" t="s">
         <v>32</v>
       </c>
       <c r="Z12" s="2"/>
@@ -2871,9 +2865,9 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="31"/>
       <c r="AF12" s="28"/>
-      <c r="AG12" s="114"/>
-    </row>
-    <row r="13" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG12" s="109"/>
+    </row>
+    <row r="13" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="104"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -2900,7 +2894,7 @@
       <c r="V13" s="28"/>
       <c r="W13" s="33"/>
       <c r="X13" s="31"/>
-      <c r="Y13" s="112"/>
+      <c r="Y13" s="108"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="41"/>
       <c r="AB13" s="2"/>
@@ -2910,7 +2904,7 @@
       <c r="AF13" s="28"/>
       <c r="AG13" s="14"/>
     </row>
-    <row r="14" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="104"/>
       <c r="B14" s="9">
         <v>0.54166666666666663</v>
@@ -2937,25 +2931,25 @@
       <c r="V14" s="28"/>
       <c r="W14" s="33"/>
       <c r="X14" s="31"/>
-      <c r="Y14" s="112" t="s">
+      <c r="Y14" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="Z14" s="113" t="s">
+      <c r="Z14" s="110" t="s">
         <v>33</v>
       </c>
       <c r="AA14" s="41"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="113" t="s">
+      <c r="AD14" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="AE14" s="113" t="s">
+      <c r="AE14" s="110" t="s">
         <v>39</v>
       </c>
       <c r="AF14" s="28"/>
       <c r="AG14" s="14"/>
     </row>
-    <row r="15" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="104"/>
       <c r="B15" s="9">
         <v>0.5625</v>
@@ -2982,17 +2976,17 @@
       <c r="V15" s="28"/>
       <c r="W15" s="33"/>
       <c r="X15" s="31"/>
-      <c r="Y15" s="112"/>
-      <c r="Z15" s="113"/>
+      <c r="Y15" s="108"/>
+      <c r="Z15" s="110"/>
       <c r="AA15" s="41"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="113"/>
-      <c r="AE15" s="113"/>
+      <c r="AD15" s="110"/>
+      <c r="AE15" s="110"/>
       <c r="AF15" s="28"/>
       <c r="AG15" s="14"/>
     </row>
-    <row r="16" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
@@ -3020,18 +3014,18 @@
       <c r="W16" s="33"/>
       <c r="X16" s="31"/>
       <c r="Y16" s="2"/>
-      <c r="Z16" s="113"/>
+      <c r="Z16" s="110"/>
       <c r="AA16" s="41"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="33"/>
-      <c r="AD16" s="113"/>
-      <c r="AE16" s="113"/>
-      <c r="AF16" s="113" t="s">
+      <c r="AD16" s="110"/>
+      <c r="AE16" s="110"/>
+      <c r="AF16" s="110" t="s">
         <v>41</v>
       </c>
       <c r="AG16" s="60"/>
     </row>
-    <row r="17" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="104"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
@@ -3043,7 +3037,7 @@
       <c r="G17" s="44"/>
       <c r="H17" s="15"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="113" t="s">
+      <c r="J17" s="110" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="28"/>
@@ -3067,10 +3061,10 @@
       <c r="AC17" s="33"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="31"/>
-      <c r="AF17" s="113"/>
+      <c r="AF17" s="110"/>
       <c r="AG17" s="60"/>
     </row>
-    <row r="18" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="104"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -3082,7 +3076,7 @@
       <c r="G18" s="44"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="113"/>
+      <c r="J18" s="110"/>
       <c r="K18" s="28"/>
       <c r="L18" s="2"/>
       <c r="M18" s="45"/>
@@ -3102,14 +3096,14 @@
       <c r="AA18" s="41"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="33"/>
-      <c r="AD18" s="112" t="s">
+      <c r="AD18" s="108" t="s">
         <v>39</v>
       </c>
       <c r="AE18" s="31"/>
-      <c r="AF18" s="113"/>
+      <c r="AF18" s="110"/>
       <c r="AG18" s="16"/>
     </row>
-    <row r="19" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="104"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
@@ -3121,7 +3115,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="113"/>
+      <c r="J19" s="110"/>
       <c r="K19" s="28"/>
       <c r="L19" s="2"/>
       <c r="M19" s="45"/>
@@ -3141,14 +3135,14 @@
       <c r="AA19" s="41"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="112"/>
-      <c r="AE19" s="112" t="s">
+      <c r="AD19" s="108"/>
+      <c r="AE19" s="108" t="s">
         <v>41</v>
       </c>
       <c r="AF19" s="28"/>
       <c r="AG19" s="16"/>
     </row>
-    <row r="20" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="104"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
@@ -3179,15 +3173,15 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="41"/>
       <c r="AB20" s="2"/>
-      <c r="AC20" s="112" t="s">
+      <c r="AC20" s="108" t="s">
         <v>34</v>
       </c>
       <c r="AD20" s="2"/>
-      <c r="AE20" s="112"/>
+      <c r="AE20" s="108"/>
       <c r="AF20" s="28"/>
       <c r="AG20" s="16"/>
     </row>
-    <row r="21" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="104"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -3218,13 +3212,13 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="41"/>
       <c r="AB21" s="2"/>
-      <c r="AC21" s="112"/>
+      <c r="AC21" s="108"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="31"/>
       <c r="AF21" s="28"/>
       <c r="AG21" s="14"/>
     </row>
-    <row r="22" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="104"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
@@ -3255,7 +3249,7 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="41"/>
       <c r="AB22" s="2"/>
-      <c r="AC22" s="112" t="s">
+      <c r="AC22" s="108" t="s">
         <v>35</v>
       </c>
       <c r="AD22" s="2"/>
@@ -3263,7 +3257,7 @@
       <c r="AF22" s="28"/>
       <c r="AG22" s="14"/>
     </row>
-    <row r="23" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="104"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
@@ -3294,13 +3288,13 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="41"/>
       <c r="AB23" s="2"/>
-      <c r="AC23" s="112"/>
+      <c r="AC23" s="108"/>
       <c r="AD23" s="2"/>
       <c r="AE23" s="31"/>
       <c r="AF23" s="28"/>
       <c r="AG23" s="14"/>
     </row>
-    <row r="24" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="104"/>
       <c r="B24" s="9">
         <v>0.75</v>
@@ -3337,7 +3331,7 @@
       <c r="AF24" s="28"/>
       <c r="AG24" s="14"/>
     </row>
-    <row r="25" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="104"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -3374,7 +3368,7 @@
       <c r="AF25" s="28"/>
       <c r="AG25" s="14"/>
     </row>
-    <row r="26" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="104"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -3411,7 +3405,7 @@
       <c r="AF26" s="28"/>
       <c r="AG26" s="14"/>
     </row>
-    <row r="27" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="105"/>
       <c r="B27" s="18">
         <v>0.812500000000001</v>
@@ -3448,7 +3442,7 @@
       <c r="AF27" s="29"/>
       <c r="AG27" s="20"/>
     </row>
-    <row r="28" spans="1:37" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="X28" s="35" t="s">
         <v>28</v>
       </c>
@@ -3456,7 +3450,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" ht="47.25" x14ac:dyDescent="0.25">
       <c r="AJ29" s="35" t="s">
         <v>29</v>
       </c>
@@ -3466,13 +3460,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="AF6:AF7"/>
-    <mergeCell ref="AG6:AG8"/>
-    <mergeCell ref="AD14:AD16"/>
-    <mergeCell ref="AD18:AD19"/>
-    <mergeCell ref="AE14:AE16"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG10:AG12"/>
     <mergeCell ref="C1:AG1"/>
     <mergeCell ref="A3:A27"/>
     <mergeCell ref="A1:B2"/>
@@ -3489,6 +3476,13 @@
     <mergeCell ref="AC20:AC21"/>
     <mergeCell ref="AE19:AE20"/>
     <mergeCell ref="AF16:AF18"/>
+    <mergeCell ref="AF6:AF7"/>
+    <mergeCell ref="AG6:AG8"/>
+    <mergeCell ref="AD14:AD16"/>
+    <mergeCell ref="AD18:AD19"/>
+    <mergeCell ref="AE14:AE16"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG10:AG12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3504,18 +3498,18 @@
       <selection activeCell="AJ35" sqref="AJ35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="10"/>
-    <col min="2" max="34" width="5.88671875" style="2" customWidth="1"/>
-    <col min="35" max="35" width="8.88671875" style="2"/>
-    <col min="36" max="36" width="44.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="10"/>
+    <col min="2" max="34" width="5.85546875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="8.85546875" style="2"/>
+    <col min="36" max="36" width="44.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="108"/>
-      <c r="B1" s="109"/>
+    <row r="1" spans="1:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="111"/>
+      <c r="B1" s="112"/>
       <c r="C1" s="98" t="s">
         <v>11</v>
       </c>
@@ -3549,9 +3543,9 @@
       <c r="AE1" s="98"/>
       <c r="AF1" s="99"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="110"/>
-      <c r="B2" s="111"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="113"/>
+      <c r="B2" s="114"/>
       <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
@@ -3649,7 +3643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="104" t="s">
         <v>6</v>
       </c>
@@ -3751,7 +3745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -3768,7 +3762,7 @@
       <c r="W4" s="61"/>
       <c r="X4" s="61"/>
       <c r="Y4" s="48"/>
-      <c r="AD4" s="113" t="s">
+      <c r="AD4" s="110" t="s">
         <v>65</v>
       </c>
       <c r="AE4" s="61"/>
@@ -3780,17 +3774,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="104"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
       </c>
       <c r="C5" s="61"/>
       <c r="D5" s="63"/>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="113" t="s">
+      <c r="F5" s="110" t="s">
         <v>42</v>
       </c>
       <c r="I5" s="61"/>
@@ -3803,7 +3797,7 @@
       <c r="W5" s="61"/>
       <c r="X5" s="61"/>
       <c r="Y5" s="48"/>
-      <c r="AD5" s="113"/>
+      <c r="AD5" s="110"/>
       <c r="AE5" s="61"/>
       <c r="AF5" s="73"/>
       <c r="AI5" s="53" t="s">
@@ -3813,50 +3807,50 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="104"/>
       <c r="B6" s="9">
         <v>0.375</v>
       </c>
       <c r="C6" s="61"/>
       <c r="D6" s="63"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="113"/>
-      <c r="I6" s="113" t="s">
+      <c r="E6" s="108"/>
+      <c r="F6" s="110"/>
+      <c r="I6" s="110" t="s">
         <v>48</v>
       </c>
       <c r="J6" s="61"/>
       <c r="K6" s="63"/>
-      <c r="L6" s="112" t="s">
+      <c r="L6" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="112" t="s">
+      <c r="M6" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="113" t="s">
+      <c r="N6" s="110" t="s">
         <v>50</v>
       </c>
       <c r="P6" s="61"/>
       <c r="Q6" s="61"/>
       <c r="R6" s="63"/>
-      <c r="S6" s="112" t="s">
+      <c r="S6" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="T6" s="113" t="s">
+      <c r="T6" s="110" t="s">
         <v>53</v>
       </c>
-      <c r="V6" s="112" t="s">
+      <c r="V6" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="W6" s="113" t="s">
+      <c r="W6" s="110" t="s">
         <v>59</v>
       </c>
       <c r="X6" s="61"/>
       <c r="Y6" s="48"/>
-      <c r="Z6" s="112" t="s">
+      <c r="Z6" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="AD6" s="113"/>
+      <c r="AD6" s="110"/>
       <c r="AE6" s="61"/>
       <c r="AF6" s="73"/>
       <c r="AI6" s="54" t="s">
@@ -3866,36 +3860,36 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="104"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="63"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="112" t="s">
+      <c r="F7" s="110"/>
+      <c r="G7" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="113" t="s">
+      <c r="H7" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="113"/>
+      <c r="I7" s="110"/>
       <c r="J7" s="61"/>
       <c r="K7" s="63"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-      <c r="N7" s="113"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="110"/>
       <c r="P7" s="61"/>
       <c r="Q7" s="61"/>
       <c r="R7" s="63"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="113"/>
-      <c r="V7" s="112"/>
-      <c r="W7" s="113"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="110"/>
+      <c r="V7" s="108"/>
+      <c r="W7" s="110"/>
       <c r="X7" s="61"/>
       <c r="Y7" s="48"/>
-      <c r="Z7" s="112"/>
+      <c r="Z7" s="108"/>
       <c r="AD7" s="61"/>
       <c r="AE7" s="61"/>
       <c r="AF7" s="73"/>
@@ -3906,40 +3900,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="104"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
       </c>
       <c r="C8" s="61"/>
       <c r="D8" s="63"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
       <c r="J8" s="61"/>
       <c r="K8" s="63"/>
       <c r="L8" s="61"/>
-      <c r="N8" s="113"/>
-      <c r="O8" s="112" t="s">
+      <c r="N8" s="110"/>
+      <c r="O8" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="110" t="s">
         <v>49</v>
       </c>
       <c r="Q8" s="61"/>
       <c r="R8" s="63"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113" t="s">
+      <c r="T8" s="110"/>
+      <c r="U8" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="W8" s="113"/>
+      <c r="W8" s="110"/>
       <c r="X8" s="61"/>
       <c r="Y8" s="48"/>
       <c r="AA8" s="16"/>
-      <c r="AB8" s="112" t="s">
+      <c r="AB8" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="AC8" s="113" t="s">
+      <c r="AC8" s="110" t="s">
         <v>56</v>
       </c>
       <c r="AD8" s="61"/>
@@ -3952,7 +3946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="104"/>
       <c r="B9" s="9">
         <v>0.4375</v>
@@ -3960,31 +3954,31 @@
       <c r="C9" s="61"/>
       <c r="D9" s="63"/>
       <c r="E9" s="59"/>
-      <c r="H9" s="113"/>
+      <c r="H9" s="110"/>
       <c r="I9" s="61"/>
       <c r="J9" s="61"/>
       <c r="K9" s="63"/>
       <c r="L9" s="61"/>
-      <c r="M9" s="112" t="s">
+      <c r="M9" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="112"/>
-      <c r="P9" s="113"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="110"/>
       <c r="Q9" s="61"/>
       <c r="R9" s="63"/>
-      <c r="S9" s="112" t="s">
+      <c r="S9" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113" t="s">
+      <c r="U9" s="110"/>
+      <c r="V9" s="110" t="s">
         <v>60</v>
       </c>
       <c r="W9" s="61"/>
       <c r="X9" s="61"/>
       <c r="Y9" s="48"/>
       <c r="AA9" s="16"/>
-      <c r="AB9" s="112"/>
-      <c r="AC9" s="113"/>
+      <c r="AB9" s="108"/>
+      <c r="AC9" s="110"/>
       <c r="AD9" s="61"/>
       <c r="AE9" s="61"/>
       <c r="AF9" s="73"/>
@@ -3995,7 +3989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="104"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
@@ -4007,29 +4001,29 @@
       <c r="J10" s="61"/>
       <c r="K10" s="63"/>
       <c r="L10" s="61"/>
-      <c r="M10" s="112"/>
-      <c r="N10" s="113" t="s">
+      <c r="M10" s="108"/>
+      <c r="N10" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="P10" s="113"/>
+      <c r="P10" s="110"/>
       <c r="Q10" s="61"/>
       <c r="R10" s="63"/>
-      <c r="S10" s="112"/>
-      <c r="T10" s="113" t="s">
+      <c r="S10" s="108"/>
+      <c r="T10" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="113"/>
-      <c r="V10" s="113"/>
+      <c r="U10" s="110"/>
+      <c r="V10" s="110"/>
       <c r="W10" s="61"/>
       <c r="X10" s="61"/>
       <c r="Y10" s="48"/>
       <c r="AA10" s="16"/>
-      <c r="AC10" s="113"/>
+      <c r="AC10" s="110"/>
       <c r="AD10" s="61"/>
       <c r="AE10" s="61"/>
       <c r="AF10" s="73"/>
     </row>
-    <row r="11" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -4037,21 +4031,21 @@
       <c r="C11" s="61"/>
       <c r="D11" s="63"/>
       <c r="E11" s="59"/>
-      <c r="H11" s="112" t="s">
+      <c r="H11" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="113" t="s">
+      <c r="I11" s="110" t="s">
         <v>47</v>
       </c>
       <c r="J11" s="61"/>
       <c r="K11" s="63"/>
       <c r="L11" s="61"/>
-      <c r="N11" s="113"/>
+      <c r="N11" s="110"/>
       <c r="P11" s="61"/>
       <c r="Q11" s="61"/>
       <c r="R11" s="63"/>
-      <c r="T11" s="113"/>
-      <c r="V11" s="113"/>
+      <c r="T11" s="110"/>
+      <c r="V11" s="110"/>
       <c r="W11" s="61"/>
       <c r="X11" s="61"/>
       <c r="Y11" s="48"/>
@@ -4060,7 +4054,7 @@
       <c r="AE11" s="61"/>
       <c r="AF11" s="73"/>
     </row>
-    <row r="12" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -4068,18 +4062,18 @@
       <c r="C12" s="61"/>
       <c r="D12" s="63"/>
       <c r="E12" s="59"/>
-      <c r="H12" s="112"/>
-      <c r="I12" s="113"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="110"/>
       <c r="J12" s="61"/>
       <c r="K12" s="63"/>
       <c r="L12" s="61"/>
-      <c r="N12" s="113"/>
-      <c r="P12" s="113" t="s">
+      <c r="N12" s="110"/>
+      <c r="P12" s="110" t="s">
         <v>66</v>
       </c>
       <c r="Q12" s="61"/>
       <c r="R12" s="63"/>
-      <c r="T12" s="113"/>
+      <c r="T12" s="110"/>
       <c r="W12" s="61"/>
       <c r="X12" s="61"/>
       <c r="Y12" s="48"/>
@@ -4088,7 +4082,7 @@
       <c r="AE12" s="61"/>
       <c r="AF12" s="73"/>
     </row>
-    <row r="13" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="104"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -4096,14 +4090,14 @@
       <c r="C13" s="61"/>
       <c r="D13" s="63"/>
       <c r="E13" s="59"/>
-      <c r="I13" s="113"/>
+      <c r="I13" s="110"/>
       <c r="J13" s="61"/>
       <c r="K13" s="63"/>
       <c r="L13" s="61"/>
-      <c r="P13" s="113"/>
+      <c r="P13" s="110"/>
       <c r="Q13" s="61"/>
       <c r="R13" s="63"/>
-      <c r="U13" s="112" t="s">
+      <c r="U13" s="108" t="s">
         <v>60</v>
       </c>
       <c r="W13" s="61"/>
@@ -4113,36 +4107,36 @@
       <c r="AE13" s="61"/>
       <c r="AF13" s="73"/>
     </row>
-    <row r="14" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="104"/>
       <c r="B14" s="9">
         <v>0.54166666666666696</v>
       </c>
       <c r="C14" s="61"/>
       <c r="D14" s="63"/>
-      <c r="F14" s="113" t="s">
+      <c r="F14" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="112" t="s">
+      <c r="H14" s="108" t="s">
         <v>48</v>
       </c>
       <c r="I14" s="61"/>
       <c r="J14" s="61"/>
       <c r="K14" s="63"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="113" t="s">
+      <c r="M14" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="N14" s="112" t="s">
+      <c r="N14" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="113" t="s">
+      <c r="O14" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="P14" s="113"/>
+      <c r="P14" s="110"/>
       <c r="Q14" s="61"/>
       <c r="R14" s="63"/>
-      <c r="U14" s="112"/>
+      <c r="U14" s="108"/>
       <c r="W14" s="61"/>
       <c r="X14" s="61"/>
       <c r="Y14" s="48"/>
@@ -4150,25 +4144,25 @@
       <c r="AE14" s="61"/>
       <c r="AF14" s="73"/>
     </row>
-    <row r="15" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="104"/>
       <c r="B15" s="9">
         <v>0.5625</v>
       </c>
       <c r="C15" s="61"/>
       <c r="D15" s="63"/>
-      <c r="E15" s="112" t="s">
+      <c r="E15" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="113"/>
-      <c r="H15" s="112"/>
+      <c r="F15" s="110"/>
+      <c r="H15" s="108"/>
       <c r="I15" s="61"/>
       <c r="J15" s="61"/>
       <c r="K15" s="63"/>
       <c r="L15" s="61"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="112"/>
-      <c r="O15" s="113"/>
+      <c r="M15" s="110"/>
+      <c r="N15" s="108"/>
+      <c r="O15" s="110"/>
       <c r="P15" s="61"/>
       <c r="Q15" s="61"/>
       <c r="R15" s="63"/>
@@ -4176,53 +4170,53 @@
       <c r="W15" s="61"/>
       <c r="X15" s="61"/>
       <c r="Y15" s="48"/>
-      <c r="AA15" s="113" t="s">
+      <c r="AA15" s="110" t="s">
         <v>57</v>
       </c>
       <c r="AD15" s="61"/>
       <c r="AE15" s="61"/>
       <c r="AF15" s="73"/>
     </row>
-    <row r="16" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
       </c>
       <c r="C16" s="61"/>
       <c r="D16" s="63"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="113"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="110"/>
       <c r="I16" s="61"/>
       <c r="J16" s="61"/>
       <c r="K16" s="63"/>
       <c r="L16" s="61"/>
-      <c r="M16" s="113"/>
-      <c r="O16" s="113"/>
+      <c r="M16" s="110"/>
+      <c r="O16" s="110"/>
       <c r="P16" s="61"/>
       <c r="Q16" s="61"/>
       <c r="R16" s="63"/>
       <c r="S16" s="30"/>
-      <c r="T16" s="112" t="s">
+      <c r="T16" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="U16" s="112" t="s">
+      <c r="U16" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="V16" s="113" t="s">
+      <c r="V16" s="110" t="s">
         <v>58</v>
       </c>
       <c r="W16" s="61"/>
       <c r="X16" s="61"/>
       <c r="Y16" s="48"/>
-      <c r="AA16" s="113"/>
-      <c r="AB16" s="112" t="s">
+      <c r="AA16" s="110"/>
+      <c r="AB16" s="108" t="s">
         <v>62</v>
       </c>
       <c r="AD16" s="61"/>
       <c r="AE16" s="61"/>
       <c r="AF16" s="73"/>
     </row>
-    <row r="17" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="104"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
@@ -4239,22 +4233,22 @@
       <c r="Q17" s="61"/>
       <c r="R17" s="63"/>
       <c r="S17" s="30"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
-      <c r="V17" s="113"/>
+      <c r="T17" s="108"/>
+      <c r="U17" s="108"/>
+      <c r="V17" s="110"/>
       <c r="W17" s="61"/>
       <c r="X17" s="61"/>
       <c r="Y17" s="48"/>
-      <c r="AA17" s="113"/>
-      <c r="AB17" s="112"/>
-      <c r="AC17" s="113" t="s">
+      <c r="AA17" s="110"/>
+      <c r="AB17" s="108"/>
+      <c r="AC17" s="110" t="s">
         <v>62</v>
       </c>
       <c r="AD17" s="61"/>
       <c r="AE17" s="61"/>
       <c r="AF17" s="73"/>
     </row>
-    <row r="18" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="104"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -4271,19 +4265,19 @@
       <c r="P18" s="16"/>
       <c r="Q18" s="61"/>
       <c r="R18" s="63"/>
-      <c r="V18" s="113"/>
+      <c r="V18" s="110"/>
       <c r="W18" s="61"/>
       <c r="X18" s="61"/>
       <c r="Y18" s="48"/>
-      <c r="Z18" s="112" t="s">
+      <c r="Z18" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="AC18" s="113"/>
+      <c r="AC18" s="110"/>
       <c r="AD18" s="61"/>
       <c r="AE18" s="61"/>
       <c r="AF18" s="73"/>
     </row>
-    <row r="19" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="104"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
@@ -4304,13 +4298,13 @@
       <c r="W19" s="61"/>
       <c r="X19" s="61"/>
       <c r="Y19" s="48"/>
-      <c r="Z19" s="112"/>
-      <c r="AC19" s="113"/>
+      <c r="Z19" s="108"/>
+      <c r="AC19" s="110"/>
       <c r="AD19" s="61"/>
       <c r="AE19" s="61"/>
       <c r="AF19" s="73"/>
     </row>
-    <row r="20" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="104"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
@@ -4331,14 +4325,14 @@
       <c r="W20" s="61"/>
       <c r="X20" s="61"/>
       <c r="Y20" s="48"/>
-      <c r="AA20" s="113" t="s">
+      <c r="AA20" s="110" t="s">
         <v>61</v>
       </c>
       <c r="AD20" s="61"/>
       <c r="AE20" s="61"/>
       <c r="AF20" s="73"/>
     </row>
-    <row r="21" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="104"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -4359,15 +4353,15 @@
       <c r="W21" s="61"/>
       <c r="X21" s="61"/>
       <c r="Y21" s="48"/>
-      <c r="AA21" s="113"/>
-      <c r="AC21" s="112" t="s">
+      <c r="AA21" s="110"/>
+      <c r="AC21" s="108" t="s">
         <v>65</v>
       </c>
       <c r="AD21" s="61"/>
       <c r="AE21" s="61"/>
       <c r="AF21" s="73"/>
     </row>
-    <row r="22" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="104"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
@@ -4381,7 +4375,7 @@
       <c r="J22" s="61"/>
       <c r="K22" s="63"/>
       <c r="L22" s="16"/>
-      <c r="O22" s="112" t="s">
+      <c r="O22" s="108" t="s">
         <v>66</v>
       </c>
       <c r="P22" s="16"/>
@@ -4390,13 +4384,13 @@
       <c r="W22" s="61"/>
       <c r="X22" s="61"/>
       <c r="Y22" s="48"/>
-      <c r="AA22" s="113"/>
-      <c r="AC22" s="112"/>
+      <c r="AA22" s="110"/>
+      <c r="AC22" s="108"/>
       <c r="AD22" s="61"/>
       <c r="AE22" s="61"/>
       <c r="AF22" s="73"/>
     </row>
-    <row r="23" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="104"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
@@ -4410,7 +4404,7 @@
       <c r="K23" s="63"/>
       <c r="L23" s="61"/>
       <c r="N23" s="61"/>
-      <c r="O23" s="112"/>
+      <c r="O23" s="108"/>
       <c r="P23" s="16"/>
       <c r="Q23" s="61"/>
       <c r="R23" s="63"/>
@@ -4425,7 +4419,7 @@
       <c r="AE23" s="61"/>
       <c r="AF23" s="73"/>
     </row>
-    <row r="24" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="104"/>
       <c r="B24" s="9">
         <v>0.75</v>
@@ -4454,7 +4448,7 @@
       <c r="AE24" s="61"/>
       <c r="AF24" s="73"/>
     </row>
-    <row r="25" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="104"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -4483,7 +4477,7 @@
       <c r="AE25" s="61"/>
       <c r="AF25" s="73"/>
     </row>
-    <row r="26" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="104"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -4512,7 +4506,7 @@
       <c r="AE26" s="61"/>
       <c r="AF26" s="73"/>
     </row>
-    <row r="27" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="105"/>
       <c r="B27" s="18">
         <v>0.812500000000001</v>
@@ -4550,21 +4544,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="U8:U10"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O16"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="AD4:AD6"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="C1:AF1"/>
+    <mergeCell ref="A3:A27"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="I6:I8"/>
     <mergeCell ref="AB16:AB17"/>
     <mergeCell ref="AC17:AC19"/>
     <mergeCell ref="AC21:AC22"/>
@@ -4581,22 +4576,21 @@
     <mergeCell ref="AA20:AA22"/>
     <mergeCell ref="V6:V7"/>
     <mergeCell ref="W6:W8"/>
-    <mergeCell ref="AD4:AD6"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="C1:AF1"/>
-    <mergeCell ref="A3:A27"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="U8:U10"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4611,18 +4605,18 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="10"/>
-    <col min="2" max="35" width="5.88671875" style="2" customWidth="1"/>
-    <col min="36" max="36" width="8.88671875" style="2"/>
-    <col min="37" max="37" width="44.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="10"/>
+    <col min="2" max="35" width="5.85546875" style="2" customWidth="1"/>
+    <col min="36" max="36" width="8.85546875" style="2"/>
+    <col min="37" max="37" width="44.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="108"/>
-      <c r="B1" s="109"/>
+    <row r="1" spans="1:37" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="111"/>
+      <c r="B1" s="112"/>
       <c r="C1" s="98" t="s">
         <v>93</v>
       </c>
@@ -4657,9 +4651,9 @@
       <c r="AF1" s="98"/>
       <c r="AG1" s="99"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A2" s="110"/>
-      <c r="B2" s="111"/>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="113"/>
+      <c r="B2" s="114"/>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
@@ -4760,7 +4754,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="104" t="s">
         <v>6</v>
       </c>
@@ -4865,7 +4859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="9">
         <v>0.33333333333333331</v>
@@ -4892,7 +4886,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="104"/>
       <c r="B5" s="9">
         <v>0.35416666666666669</v>
@@ -4919,13 +4913,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="104"/>
       <c r="B6" s="9">
         <v>0.375</v>
       </c>
       <c r="C6" s="61"/>
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="110" t="s">
         <v>63</v>
       </c>
       <c r="I6" s="63"/>
@@ -4948,13 +4942,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104"/>
       <c r="B7" s="9">
         <v>0.39583333333333298</v>
       </c>
       <c r="C7" s="61"/>
-      <c r="D7" s="113"/>
+      <c r="D7" s="110"/>
       <c r="I7" s="63"/>
       <c r="J7" s="61"/>
       <c r="K7" s="61"/>
@@ -4975,17 +4969,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="104"/>
       <c r="B8" s="9">
         <v>0.41666666666666702</v>
       </c>
       <c r="C8" s="61"/>
-      <c r="D8" s="113"/>
-      <c r="F8" s="112" t="s">
+      <c r="D8" s="110"/>
+      <c r="F8" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="113" t="s">
+      <c r="G8" s="110" t="s">
         <v>67</v>
       </c>
       <c r="I8" s="63"/>
@@ -5002,15 +4996,15 @@
       <c r="AF8" s="61"/>
       <c r="AG8" s="14"/>
     </row>
-    <row r="9" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104"/>
       <c r="B9" s="9">
         <v>0.4375</v>
       </c>
       <c r="C9" s="61"/>
       <c r="D9" s="61"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="110"/>
       <c r="I9" s="63"/>
       <c r="J9" s="61"/>
       <c r="K9" s="61"/>
@@ -5025,14 +5019,14 @@
       <c r="AF9" s="61"/>
       <c r="AG9" s="14"/>
     </row>
-    <row r="10" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="104"/>
       <c r="B10" s="9">
         <v>0.45833333333333298</v>
       </c>
       <c r="C10" s="61"/>
       <c r="D10" s="61"/>
-      <c r="G10" s="113"/>
+      <c r="G10" s="110"/>
       <c r="I10" s="63"/>
       <c r="J10" s="61"/>
       <c r="K10" s="61"/>
@@ -5047,7 +5041,7 @@
       <c r="AF10" s="61"/>
       <c r="AG10" s="14"/>
     </row>
-    <row r="11" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104"/>
       <c r="B11" s="9">
         <v>0.47916666666666702</v>
@@ -5068,7 +5062,7 @@
       <c r="AF11" s="61"/>
       <c r="AG11" s="14"/>
     </row>
-    <row r="12" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104"/>
       <c r="B12" s="9">
         <v>0.5</v>
@@ -5089,7 +5083,7 @@
       <c r="AF12" s="61"/>
       <c r="AG12" s="14"/>
     </row>
-    <row r="13" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="104"/>
       <c r="B13" s="9">
         <v>0.52083333333333304</v>
@@ -5110,7 +5104,7 @@
       <c r="AF13" s="61"/>
       <c r="AG13" s="14"/>
     </row>
-    <row r="14" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="104"/>
       <c r="B14" s="9">
         <v>0.54166666666666696</v>
@@ -5131,16 +5125,16 @@
       <c r="AF14" s="61"/>
       <c r="AG14" s="14"/>
     </row>
-    <row r="15" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="104"/>
       <c r="B15" s="9">
         <v>0.5625</v>
       </c>
       <c r="C15" s="33"/>
-      <c r="D15" s="112" t="s">
+      <c r="D15" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="113" t="s">
+      <c r="E15" s="110" t="s">
         <v>64</v>
       </c>
       <c r="I15" s="63"/>
@@ -5157,14 +5151,14 @@
       <c r="AF15" s="61"/>
       <c r="AG15" s="14"/>
     </row>
-    <row r="16" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
       <c r="B16" s="9">
         <v>0.58333333333333304</v>
       </c>
       <c r="C16" s="33"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="113"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="110"/>
       <c r="I16" s="63"/>
       <c r="J16" s="61"/>
       <c r="K16" s="61"/>
@@ -5179,14 +5173,14 @@
       <c r="AF16" s="61"/>
       <c r="AG16" s="14"/>
     </row>
-    <row r="17" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="104"/>
       <c r="B17" s="9">
         <v>0.60416666666666696</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="61"/>
-      <c r="E17" s="113"/>
+      <c r="E17" s="110"/>
       <c r="I17" s="63"/>
       <c r="J17" s="61"/>
       <c r="K17" s="61"/>
@@ -5201,7 +5195,7 @@
       <c r="AF17" s="61"/>
       <c r="AG17" s="14"/>
     </row>
-    <row r="18" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="104"/>
       <c r="B18" s="9">
         <v>0.625</v>
@@ -5222,12 +5216,12 @@
       <c r="AF18" s="61"/>
       <c r="AG18" s="14"/>
     </row>
-    <row r="19" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="104"/>
       <c r="B19" s="9">
         <v>0.64583333333333404</v>
       </c>
-      <c r="C19" s="112" t="s">
+      <c r="C19" s="108" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="61"/>
@@ -5245,12 +5239,12 @@
       <c r="AF19" s="61"/>
       <c r="AG19" s="14"/>
     </row>
-    <row r="20" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="104"/>
       <c r="B20" s="9">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C20" s="112"/>
+      <c r="C20" s="108"/>
       <c r="D20" s="61"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -5269,7 +5263,7 @@
       <c r="AF20" s="61"/>
       <c r="AG20" s="14"/>
     </row>
-    <row r="21" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="104"/>
       <c r="B21" s="9">
         <v>0.6875</v>
@@ -5293,15 +5287,15 @@
       <c r="AF21" s="61"/>
       <c r="AG21" s="14"/>
     </row>
-    <row r="22" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="104"/>
       <c r="B22" s="9">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C22" s="112" t="s">
+      <c r="C22" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="113" t="s">
+      <c r="D22" s="110" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="16"/>
@@ -5321,13 +5315,13 @@
       <c r="AF22" s="61"/>
       <c r="AG22" s="14"/>
     </row>
-    <row r="23" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="104"/>
       <c r="B23" s="9">
         <v>0.72916666666666696</v>
       </c>
-      <c r="C23" s="112"/>
-      <c r="D23" s="113"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="110"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
@@ -5352,13 +5346,13 @@
       <c r="AF23" s="61"/>
       <c r="AG23" s="14"/>
     </row>
-    <row r="24" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="104"/>
       <c r="B24" s="9">
         <v>0.75</v>
       </c>
       <c r="C24" s="61"/>
-      <c r="D24" s="113"/>
+      <c r="D24" s="110"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
@@ -5383,7 +5377,7 @@
       <c r="AF24" s="61"/>
       <c r="AG24" s="14"/>
     </row>
-    <row r="25" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="104"/>
       <c r="B25" s="9">
         <v>0.77083333333333404</v>
@@ -5414,7 +5408,7 @@
       <c r="AF25" s="61"/>
       <c r="AG25" s="14"/>
     </row>
-    <row r="26" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="104"/>
       <c r="B26" s="9">
         <v>0.79166666666666696</v>
@@ -5445,7 +5439,7 @@
       <c r="AF26" s="61"/>
       <c r="AG26" s="14"/>
     </row>
-    <row r="27" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="105"/>
       <c r="B27" s="18">
         <v>0.812500000000001</v>
@@ -5509,30 +5503,30 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="82" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="48.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="185.88671875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="10.6640625" style="2" customWidth="1"/>
-    <col min="13" max="15" width="12.109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="8.88671875" style="2"/>
-    <col min="21" max="21" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="82" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="48.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="185.85546875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" style="2" customWidth="1"/>
+    <col min="13" max="15" width="12.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="8.85546875" style="2"/>
+    <col min="21" max="21" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="76" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="76" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="76" t="s">
         <v>36</v>
       </c>
@@ -5579,7 +5573,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -5626,7 +5620,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -5673,7 +5667,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -5723,7 +5717,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -5764,7 +5758,7 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -5813,7 +5807,7 @@
       <c r="V6" s="116"/>
       <c r="W6" s="117"/>
     </row>
-    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -5864,7 +5858,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -5916,7 +5910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -5968,7 +5962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -6020,7 +6014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -6072,7 +6066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -6127,7 +6121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
@@ -6182,7 +6176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -6220,7 +6214,7 @@
         <v>81.099999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="70" t="s">
         <v>47</v>
       </c>
@@ -6267,7 +6261,7 @@
       <c r="W15" s="116"/>
       <c r="X15" s="117"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="s">
         <v>48</v>
       </c>
@@ -6320,7 +6314,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -6373,7 +6367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -6432,7 +6426,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
@@ -6485,7 +6479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -6529,7 +6523,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -6573,7 +6567,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
@@ -6614,7 +6608,7 @@
         <v>58.6</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -6652,7 +6646,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -6690,7 +6684,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -6731,7 +6725,7 @@
         <v>76.900000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
@@ -6775,7 +6769,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -6819,7 +6813,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
@@ -6863,7 +6857,7 @@
         <v>84.2</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
@@ -6901,7 +6895,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
@@ -6939,7 +6933,7 @@
         <v>60.2</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
@@ -6980,7 +6974,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -7021,7 +7015,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
@@ -7059,7 +7053,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -7097,7 +7091,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -7138,7 +7132,7 @@
         <v>72.099999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
@@ -7179,7 +7173,7 @@
         <v>111.1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -7234,33 +7228,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A5247D-4E00-4B4A-AEA2-655372E0F049}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="93" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" style="93" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="93" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="94" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="93" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="93" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="93" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" style="93" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" style="93" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="9.109375" style="93" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" style="93" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.77734375" style="93" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" style="93" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" style="2"/>
+    <col min="4" max="7" width="13.7109375" style="93"/>
+    <col min="8" max="8" width="13.7109375" style="94"/>
+    <col min="9" max="18" width="13.7109375" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="97" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
         <v>36</v>
       </c>
@@ -7289,43 +7271,37 @@
         <v>137</v>
       </c>
       <c r="J1" s="95" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="K1" s="95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L1" s="95" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="N1" s="95" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O1" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P1" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q1" s="95" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="95" t="s">
         <v>110</v>
       </c>
+      <c r="R1" s="97" t="s">
+        <v>135</v>
+      </c>
       <c r="S1" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="T1" s="97" t="s">
-        <v>135</v>
-      </c>
-      <c r="U1" s="95" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -7353,38 +7329,38 @@
       <c r="I2" s="93">
         <v>0.4152777777777778</v>
       </c>
+      <c r="J2" s="93">
+        <v>0.4284722222222222</v>
+      </c>
       <c r="K2" s="93">
-        <v>0.4284722222222222</v>
+        <v>0.43611111111111112</v>
       </c>
       <c r="L2" s="93">
-        <v>0.43611111111111112</v>
+        <v>0.43888888888888888</v>
       </c>
       <c r="M2" s="93">
-        <v>0.43888888888888888</v>
+        <v>0.44305555555555554</v>
       </c>
       <c r="N2" s="93">
-        <v>0.44305555555555554</v>
+        <v>0.44930555555555557</v>
       </c>
       <c r="O2" s="93">
-        <v>0.44930555555555557</v>
+        <v>0.45416666666666666</v>
       </c>
       <c r="P2" s="93">
-        <v>0.45416666666666666</v>
+        <v>0.45902777777777776</v>
       </c>
       <c r="Q2" s="93">
-        <v>0.45902777777777776</v>
+        <v>0.46458333333333335</v>
       </c>
       <c r="R2" s="93">
-        <v>0.46458333333333335</v>
-      </c>
-      <c r="T2" s="93">
         <v>0.47083333333333333</v>
       </c>
-      <c r="U2" s="92">
+      <c r="S2" s="92">
         <v>0.4861111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -7412,38 +7388,38 @@
       <c r="I3" s="93">
         <v>0.56111111111111112</v>
       </c>
+      <c r="J3" s="93">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="K3" s="93">
-        <v>0.57291666666666663</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="L3" s="93">
-        <v>0.57499999999999996</v>
+        <v>0.57847222222222228</v>
       </c>
       <c r="M3" s="93">
-        <v>0.57847222222222228</v>
+        <v>0.58125000000000004</v>
       </c>
       <c r="N3" s="93">
-        <v>0.58125000000000004</v>
+        <v>0.58680555555555558</v>
       </c>
       <c r="O3" s="93">
-        <v>0.58680555555555558</v>
+        <v>0.59166666666666667</v>
       </c>
       <c r="P3" s="93">
-        <v>0.59166666666666667</v>
+        <v>0.59652777777777777</v>
       </c>
       <c r="Q3" s="93">
-        <v>0.59652777777777777</v>
+        <v>0.60138888888888886</v>
       </c>
       <c r="R3" s="93">
-        <v>0.60138888888888886</v>
-      </c>
-      <c r="T3" s="93">
         <v>0.6069444444444444</v>
       </c>
-      <c r="U3" s="92">
+      <c r="S3" s="92">
         <v>0.61805555555555558</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -7471,38 +7447,38 @@
       <c r="I4" s="93">
         <v>0.375</v>
       </c>
+      <c r="J4" s="93">
+        <v>0.39513888888888887</v>
+      </c>
       <c r="K4" s="93">
-        <v>0.39513888888888887</v>
+        <v>0.3972222222222222</v>
       </c>
       <c r="L4" s="93">
-        <v>0.3972222222222222</v>
+        <v>0.40069444444444446</v>
       </c>
       <c r="M4" s="93">
-        <v>0.40069444444444446</v>
+        <v>0.40416666666666667</v>
       </c>
       <c r="N4" s="93">
-        <v>0.40416666666666667</v>
+        <v>0.40902777777777777</v>
       </c>
       <c r="O4" s="93">
-        <v>0.40902777777777777</v>
+        <v>0.41388888888888886</v>
       </c>
       <c r="P4" s="93">
-        <v>0.41388888888888886</v>
+        <v>0.41875000000000001</v>
       </c>
       <c r="Q4" s="93">
-        <v>0.41875000000000001</v>
+        <v>0.42430555555555555</v>
       </c>
       <c r="R4" s="93">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="T4" s="93">
         <v>0.42986111111111114</v>
       </c>
-      <c r="U4" s="92">
+      <c r="S4" s="92">
         <v>0.4375</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -7530,38 +7506,38 @@
       <c r="I5" s="93">
         <v>0.54166666666666663</v>
       </c>
+      <c r="J5" s="93">
+        <v>0.56111111111111112</v>
+      </c>
       <c r="K5" s="93">
-        <v>0.56111111111111112</v>
+        <v>0.5625</v>
       </c>
       <c r="L5" s="93">
-        <v>0.5625</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="M5" s="93">
-        <v>0.56666666666666665</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="N5" s="93">
-        <v>0.56944444444444442</v>
+        <v>0.57430555555555551</v>
       </c>
       <c r="O5" s="93">
-        <v>0.57430555555555551</v>
+        <v>0.57916666666666672</v>
       </c>
       <c r="P5" s="93">
-        <v>0.57916666666666672</v>
+        <v>0.58402777777777781</v>
       </c>
       <c r="Q5" s="93">
-        <v>0.58402777777777781</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="R5" s="93">
-        <v>0.58819444444444446</v>
-      </c>
-      <c r="T5" s="93">
         <v>0.59444444444444444</v>
       </c>
-      <c r="U5" s="92">
+      <c r="S5" s="92">
         <v>0.60069444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -7589,38 +7565,38 @@
       <c r="I6" s="93">
         <v>0.5395833333333333</v>
       </c>
+      <c r="J6" s="93">
+        <v>0.55347222222222225</v>
+      </c>
       <c r="K6" s="93">
-        <v>0.55347222222222225</v>
+        <v>0.5541666666666667</v>
       </c>
       <c r="L6" s="93">
-        <v>0.5541666666666667</v>
+        <v>0.55763888888888891</v>
       </c>
       <c r="M6" s="93">
-        <v>0.55763888888888891</v>
+        <v>0.56111111111111112</v>
       </c>
       <c r="N6" s="93">
-        <v>0.56111111111111112</v>
+        <v>0.56597222222222221</v>
       </c>
       <c r="O6" s="93">
-        <v>0.56597222222222221</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="P6" s="93">
-        <v>0.57291666666666663</v>
+        <v>0.57777777777777772</v>
       </c>
       <c r="Q6" s="93">
-        <v>0.57777777777777772</v>
+        <v>0.58263888888888893</v>
       </c>
       <c r="R6" s="93">
-        <v>0.58263888888888893</v>
-      </c>
-      <c r="T6" s="93">
         <v>0.58888888888888891</v>
       </c>
-      <c r="U6" s="92">
+      <c r="S6" s="92">
         <v>0.59861111111111109</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -7648,38 +7624,38 @@
       <c r="I7" s="93">
         <v>0.40208333333333335</v>
       </c>
+      <c r="J7" s="93">
+        <v>0.41388888888888886</v>
+      </c>
       <c r="K7" s="93">
-        <v>0.41388888888888886</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="L7" s="93">
-        <v>0.4152777777777778</v>
+        <v>0.41875000000000001</v>
       </c>
       <c r="M7" s="93">
-        <v>0.41875000000000001</v>
+        <v>0.42222222222222222</v>
       </c>
       <c r="N7" s="93">
-        <v>0.42222222222222222</v>
+        <v>0.42777777777777776</v>
       </c>
       <c r="O7" s="93">
-        <v>0.42777777777777776</v>
+        <v>0.43263888888888891</v>
       </c>
       <c r="P7" s="93">
-        <v>0.43263888888888891</v>
+        <v>0.43819444444444444</v>
       </c>
       <c r="Q7" s="93">
-        <v>0.43819444444444444</v>
+        <v>0.44374999999999998</v>
       </c>
       <c r="R7" s="93">
-        <v>0.44374999999999998</v>
-      </c>
-      <c r="T7" s="93">
         <v>0.45624999999999999</v>
       </c>
-      <c r="U7" s="92">
+      <c r="S7" s="92">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -7707,38 +7683,38 @@
       <c r="I8" s="93">
         <v>0.54513888888888884</v>
       </c>
+      <c r="J8" s="93">
+        <v>0.56458333333333333</v>
+      </c>
       <c r="K8" s="93">
-        <v>0.56458333333333333</v>
+        <v>0.56597222222222221</v>
       </c>
       <c r="L8" s="93">
-        <v>0.56597222222222221</v>
+        <v>0.57708333333333328</v>
       </c>
       <c r="M8" s="93">
-        <v>0.57708333333333328</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="N8" s="93">
-        <v>0.58819444444444446</v>
+        <v>0.59375</v>
       </c>
       <c r="O8" s="93">
-        <v>0.59375</v>
+        <v>0.59930555555555554</v>
       </c>
       <c r="P8" s="93">
-        <v>0.59930555555555554</v>
+        <v>0.60486111111111107</v>
       </c>
       <c r="Q8" s="93">
-        <v>0.60486111111111107</v>
+        <v>0.61041666666666672</v>
       </c>
       <c r="R8" s="93">
-        <v>0.61041666666666672</v>
-      </c>
-      <c r="T8" s="93">
         <v>0.61736111111111114</v>
       </c>
-      <c r="U8" s="92">
+      <c r="S8" s="92">
         <v>0.62152777777777779</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -7766,38 +7742,38 @@
       <c r="I9" s="93">
         <v>0.375</v>
       </c>
+      <c r="J9" s="93">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="K9" s="93">
-        <v>0.39583333333333331</v>
+        <v>0.3972222222222222</v>
       </c>
       <c r="L9" s="93">
-        <v>0.3972222222222222</v>
+        <v>0.40069444444444446</v>
       </c>
       <c r="M9" s="93">
-        <v>0.40069444444444446</v>
+        <v>0.40416666666666667</v>
       </c>
       <c r="N9" s="93">
-        <v>0.40416666666666667</v>
+        <v>0.40972222222222221</v>
       </c>
       <c r="O9" s="93">
-        <v>0.40972222222222221</v>
+        <v>0.41597222222222224</v>
       </c>
       <c r="P9" s="93">
-        <v>0.41597222222222224</v>
+        <v>0.42152777777777778</v>
       </c>
       <c r="Q9" s="93">
-        <v>0.42152777777777778</v>
+        <v>0.42638888888888887</v>
       </c>
       <c r="R9" s="93">
-        <v>0.42638888888888887</v>
-      </c>
-      <c r="T9" s="93">
         <v>0.43194444444444446</v>
       </c>
-      <c r="U9" s="92">
+      <c r="S9" s="92">
         <v>0.4513888888888889</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -7825,38 +7801,38 @@
       <c r="I10" s="93">
         <v>0.58333333333333337</v>
       </c>
+      <c r="J10" s="93">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="K10" s="93">
-        <v>0.60416666666666663</v>
+        <v>0.60555555555555551</v>
       </c>
       <c r="L10" s="93">
-        <v>0.60555555555555551</v>
+        <v>0.60902777777777772</v>
       </c>
       <c r="M10" s="93">
-        <v>0.60902777777777772</v>
-      </c>
-      <c r="N10" s="93">
         <v>0.61250000000000004</v>
       </c>
-      <c r="O10" s="92">
+      <c r="N10" s="92">
         <v>0.61736111111111114</v>
       </c>
+      <c r="O10" s="93">
+        <v>0.62291666666666667</v>
+      </c>
       <c r="P10" s="93">
-        <v>0.62291666666666667</v>
+        <v>0.62986111111111109</v>
       </c>
       <c r="Q10" s="93">
-        <v>0.62986111111111109</v>
+        <v>0.63680555555555551</v>
       </c>
       <c r="R10" s="93">
-        <v>0.63680555555555551</v>
-      </c>
-      <c r="T10" s="93">
         <v>0.6430555555555556</v>
       </c>
-      <c r="U10" s="92">
+      <c r="S10" s="92">
         <v>0.65972222222222221</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -7884,38 +7860,38 @@
       <c r="I11" s="93">
         <v>0.35416666666666669</v>
       </c>
+      <c r="J11" s="93">
+        <v>0.37013888888888891</v>
+      </c>
       <c r="K11" s="93">
-        <v>0.37013888888888891</v>
+        <v>0.37152777777777779</v>
       </c>
       <c r="L11" s="93">
-        <v>0.37152777777777779</v>
+        <v>0.375</v>
       </c>
       <c r="M11" s="93">
-        <v>0.375</v>
+        <v>0.37986111111111109</v>
       </c>
       <c r="N11" s="93">
-        <v>0.37986111111111109</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="O11" s="93">
-        <v>0.38541666666666669</v>
+        <v>0.39027777777777778</v>
       </c>
       <c r="P11" s="93">
-        <v>0.39027777777777778</v>
+        <v>0.39513888888888887</v>
       </c>
       <c r="Q11" s="93">
-        <v>0.39513888888888887</v>
+        <v>0.4</v>
       </c>
       <c r="R11" s="93">
-        <v>0.4</v>
-      </c>
-      <c r="T11" s="93">
         <v>0.40694444444444444</v>
       </c>
-      <c r="U11" s="92">
+      <c r="S11" s="92">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -7943,38 +7919,38 @@
       <c r="I12" s="93">
         <v>0.54166666666666663</v>
       </c>
+      <c r="J12" s="93">
+        <v>0.56180555555555556</v>
+      </c>
       <c r="K12" s="93">
-        <v>0.56180555555555556</v>
+        <v>0.56319444444444444</v>
       </c>
       <c r="L12" s="93">
-        <v>0.56319444444444444</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="M12" s="93">
-        <v>0.56666666666666665</v>
+        <v>0.57013888888888886</v>
       </c>
       <c r="N12" s="93">
-        <v>0.57013888888888886</v>
+        <v>0.57638888888888884</v>
       </c>
       <c r="O12" s="93">
-        <v>0.57638888888888884</v>
+        <v>0.58263888888888893</v>
       </c>
       <c r="P12" s="93">
-        <v>0.58263888888888893</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="Q12" s="93">
-        <v>0.58819444444444446</v>
+        <v>0.59375</v>
       </c>
       <c r="R12" s="93">
-        <v>0.59375</v>
-      </c>
-      <c r="T12" s="93">
         <v>0.60138888888888886</v>
       </c>
-      <c r="U12" s="92">
+      <c r="S12" s="92">
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -8002,38 +7978,38 @@
       <c r="I13" s="93">
         <v>0.39374999999999999</v>
       </c>
+      <c r="J13" s="93">
+        <v>0.4152777777777778</v>
+      </c>
       <c r="K13" s="93">
-        <v>0.4152777777777778</v>
+        <v>0.41597222222222224</v>
       </c>
       <c r="L13" s="93">
-        <v>0.41597222222222224</v>
+        <v>0.41944444444444445</v>
       </c>
       <c r="M13" s="93">
-        <v>0.41944444444444445</v>
+        <v>0.42291666666666666</v>
       </c>
       <c r="N13" s="93">
-        <v>0.42291666666666666</v>
+        <v>0.42777777777777776</v>
       </c>
       <c r="O13" s="93">
-        <v>0.42777777777777776</v>
+        <v>0.43194444444444446</v>
       </c>
       <c r="P13" s="93">
-        <v>0.43194444444444446</v>
+        <v>0.4375</v>
       </c>
       <c r="Q13" s="93">
-        <v>0.4375</v>
+        <v>0.44236111111111109</v>
       </c>
       <c r="R13" s="93">
-        <v>0.44236111111111109</v>
-      </c>
-      <c r="T13" s="93">
         <v>0.44930555555555557</v>
       </c>
-      <c r="U13" s="92">
+      <c r="S13" s="92">
         <v>0.45624999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -8061,38 +8037,38 @@
       <c r="I14" s="93">
         <v>0.45833333333333331</v>
       </c>
+      <c r="J14" s="93">
+        <v>0.47083333333333333</v>
+      </c>
       <c r="K14" s="93">
-        <v>0.47083333333333333</v>
+        <v>0.47291666666666665</v>
       </c>
       <c r="L14" s="93">
-        <v>0.47291666666666665</v>
+        <v>0.47708333333333336</v>
       </c>
       <c r="M14" s="93">
-        <v>0.47708333333333336</v>
+        <v>0.47986111111111113</v>
       </c>
       <c r="N14" s="93">
-        <v>0.47986111111111113</v>
+        <v>0.48472222222222222</v>
       </c>
       <c r="O14" s="93">
-        <v>0.48472222222222222</v>
+        <v>0.49027777777777776</v>
       </c>
       <c r="P14" s="93">
-        <v>0.49027777777777776</v>
+        <v>0.49513888888888891</v>
       </c>
       <c r="Q14" s="93">
-        <v>0.49513888888888891</v>
+        <v>0.5</v>
       </c>
       <c r="R14" s="93">
-        <v>0.5</v>
-      </c>
-      <c r="T14" s="93">
         <v>0.50624999999999998</v>
       </c>
-      <c r="U14" s="92">
+      <c r="S14" s="92">
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -8120,38 +8096,38 @@
       <c r="I15" s="93">
         <v>0.54166666666666663</v>
       </c>
+      <c r="J15" s="93">
+        <v>0.55486111111111114</v>
+      </c>
       <c r="K15" s="93">
-        <v>0.55486111111111114</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="L15" s="93">
-        <v>0.55555555555555558</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="M15" s="93">
-        <v>0.55902777777777779</v>
+        <v>0.5625</v>
       </c>
       <c r="N15" s="93">
-        <v>0.5625</v>
+        <v>0.56736111111111109</v>
       </c>
       <c r="O15" s="93">
-        <v>0.56736111111111109</v>
+        <v>0.57222222222222219</v>
       </c>
       <c r="P15" s="93">
-        <v>0.57222222222222219</v>
+        <v>0.57638888888888884</v>
       </c>
       <c r="Q15" s="93">
-        <v>0.57638888888888884</v>
+        <v>0.58194444444444449</v>
       </c>
       <c r="R15" s="93">
-        <v>0.58194444444444449</v>
-      </c>
-      <c r="T15" s="93">
         <v>0.59027777777777779</v>
       </c>
-      <c r="U15" s="92">
+      <c r="S15" s="92">
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="s">
         <v>47</v>
       </c>
@@ -8179,38 +8155,38 @@
       <c r="I16" s="93">
         <v>0.48055555555555557</v>
       </c>
+      <c r="J16" s="93">
+        <v>0.4909722222222222</v>
+      </c>
       <c r="K16" s="93">
-        <v>0.4909722222222222</v>
+        <v>0.49166666666666664</v>
       </c>
       <c r="L16" s="93">
-        <v>0.49166666666666664</v>
+        <v>0.49513888888888891</v>
       </c>
       <c r="M16" s="93">
-        <v>0.49513888888888891</v>
+        <v>0.49791666666666667</v>
       </c>
       <c r="N16" s="93">
-        <v>0.49791666666666667</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="O16" s="93">
-        <v>0.50347222222222221</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="P16" s="93">
-        <v>0.5083333333333333</v>
+        <v>0.51388888888888884</v>
       </c>
       <c r="Q16" s="93">
-        <v>0.51388888888888884</v>
+        <v>0.51875000000000004</v>
       </c>
       <c r="R16" s="93">
-        <v>0.51875000000000004</v>
-      </c>
-      <c r="T16" s="93">
         <v>0.52430555555555558</v>
       </c>
-      <c r="U16" s="92">
+      <c r="S16" s="92">
         <v>0.53263888888888888</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
         <v>48</v>
       </c>
@@ -8238,38 +8214,38 @@
       <c r="I17" s="93">
         <v>0.375</v>
       </c>
+      <c r="J17" s="93">
+        <v>0.38680555555555557</v>
+      </c>
       <c r="K17" s="93">
-        <v>0.38680555555555557</v>
+        <v>0.38819444444444445</v>
       </c>
       <c r="L17" s="93">
-        <v>0.38819444444444445</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="M17" s="93">
-        <v>0.39097222222222222</v>
+        <v>0.3972222222222222</v>
       </c>
       <c r="N17" s="93">
-        <v>0.3972222222222222</v>
+        <v>0.40208333333333335</v>
       </c>
       <c r="O17" s="93">
-        <v>0.40208333333333335</v>
+        <v>0.40694444444444444</v>
       </c>
       <c r="P17" s="93">
-        <v>0.40694444444444444</v>
+        <v>0.41249999999999998</v>
       </c>
       <c r="Q17" s="93">
-        <v>0.41249999999999998</v>
+        <v>0.41736111111111113</v>
       </c>
       <c r="R17" s="93">
-        <v>0.41736111111111113</v>
-      </c>
-      <c r="T17" s="93">
         <v>0.42430555555555555</v>
       </c>
-      <c r="U17" s="92">
+      <c r="S17" s="92">
         <v>0.43402777777777779</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -8297,38 +8273,38 @@
       <c r="I18" s="93">
         <v>0.43402777777777779</v>
       </c>
+      <c r="J18" s="93">
+        <v>0.45208333333333334</v>
+      </c>
       <c r="K18" s="93">
-        <v>0.45208333333333334</v>
+        <v>0.45347222222222222</v>
       </c>
       <c r="L18" s="93">
-        <v>0.45347222222222222</v>
+        <v>0.45624999999999999</v>
       </c>
       <c r="M18" s="93">
-        <v>0.45624999999999999</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="N18" s="93">
-        <v>0.4597222222222222</v>
+        <v>0.46597222222222223</v>
       </c>
       <c r="O18" s="93">
-        <v>0.46597222222222223</v>
+        <v>0.47083333333333333</v>
       </c>
       <c r="P18" s="93">
-        <v>0.47083333333333333</v>
+        <v>0.47638888888888886</v>
       </c>
       <c r="Q18" s="93">
-        <v>0.47638888888888886</v>
+        <v>0.48125000000000001</v>
       </c>
       <c r="R18" s="93">
-        <v>0.48125000000000001</v>
-      </c>
-      <c r="T18" s="93">
         <v>0.48888888888888887</v>
       </c>
-      <c r="U18" s="92">
+      <c r="S18" s="92">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -8356,38 +8332,38 @@
       <c r="I19" s="93">
         <v>0.37152777777777779</v>
       </c>
+      <c r="J19" s="93">
+        <v>0.38958333333333334</v>
+      </c>
       <c r="K19" s="93">
-        <v>0.38958333333333334</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="L19" s="93">
-        <v>0.39097222222222222</v>
+        <v>0.39444444444444443</v>
       </c>
       <c r="M19" s="93">
-        <v>0.39444444444444443</v>
+        <v>0.3972222222222222</v>
       </c>
       <c r="N19" s="93">
-        <v>0.3972222222222222</v>
+        <v>0.40208333333333335</v>
       </c>
       <c r="O19" s="93">
-        <v>0.40208333333333335</v>
+        <v>0.40694444444444444</v>
       </c>
       <c r="P19" s="93">
-        <v>0.40694444444444444</v>
+        <v>0.41180555555555554</v>
       </c>
       <c r="Q19" s="93">
-        <v>0.41180555555555554</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="R19" s="93">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="T19" s="93">
         <v>0.42430555555555555</v>
       </c>
-      <c r="U19" s="92">
+      <c r="S19" s="92">
         <v>0.4375</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -8415,38 +8391,38 @@
       <c r="I20" s="93">
         <v>0.53819444444444442</v>
       </c>
+      <c r="J20" s="93">
+        <v>0.55833333333333335</v>
+      </c>
       <c r="K20" s="93">
-        <v>0.55833333333333335</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="L20" s="93">
-        <v>0.55902777777777779</v>
+        <v>0.5625</v>
       </c>
       <c r="M20" s="93">
-        <v>0.5625</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="N20" s="93">
-        <v>0.56666666666666665</v>
+        <v>0.57152777777777775</v>
       </c>
       <c r="O20" s="93">
-        <v>0.57152777777777775</v>
+        <v>0.57638888888888884</v>
       </c>
       <c r="P20" s="93">
-        <v>0.57638888888888884</v>
+        <v>0.58125000000000004</v>
       </c>
       <c r="Q20" s="93">
-        <v>0.58125000000000004</v>
+        <v>0.58611111111111114</v>
       </c>
       <c r="R20" s="93">
-        <v>0.58611111111111114</v>
-      </c>
-      <c r="T20" s="93">
         <v>0.59236111111111112</v>
       </c>
-      <c r="U20" s="92">
+      <c r="S20" s="92">
         <v>0.60069444444444442</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -8474,38 +8450,38 @@
       <c r="I21" s="93">
         <v>0.47152777777777777</v>
       </c>
+      <c r="J21" s="93">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="K21" s="93">
-        <v>0.4826388888888889</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="L21" s="93">
-        <v>0.48333333333333334</v>
+        <v>0.48680555555555555</v>
       </c>
       <c r="M21" s="93">
-        <v>0.48680555555555555</v>
+        <v>0.49027777777777776</v>
       </c>
       <c r="N21" s="93">
-        <v>0.49027777777777776</v>
+        <v>0.49513888888888891</v>
       </c>
       <c r="O21" s="93">
-        <v>0.49513888888888891</v>
+        <v>0.5</v>
       </c>
       <c r="P21" s="93">
-        <v>0.5</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="Q21" s="93">
-        <v>0.50486111111111109</v>
+        <v>0.50972222222222219</v>
       </c>
       <c r="R21" s="93">
-        <v>0.50972222222222219</v>
-      </c>
-      <c r="T21" s="93">
         <v>0.51458333333333328</v>
       </c>
-      <c r="U21" s="92">
+      <c r="S21" s="92">
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -8533,38 +8509,38 @@
       <c r="I22" s="93">
         <v>0.37777777777777777</v>
       </c>
+      <c r="J22" s="93">
+        <v>0.39166666666666666</v>
+      </c>
       <c r="K22" s="93">
-        <v>0.39166666666666666</v>
+        <v>0.39374999999999999</v>
       </c>
       <c r="L22" s="93">
-        <v>0.39374999999999999</v>
+        <v>0.3972222222222222</v>
       </c>
       <c r="M22" s="93">
-        <v>0.3972222222222222</v>
+        <v>0.40069444444444446</v>
       </c>
       <c r="N22" s="93">
-        <v>0.40069444444444446</v>
+        <v>0.40694444444444444</v>
       </c>
       <c r="O22" s="93">
-        <v>0.40694444444444444</v>
+        <v>0.41249999999999998</v>
       </c>
       <c r="P22" s="93">
-        <v>0.41249999999999998</v>
+        <v>0.41805555555555557</v>
       </c>
       <c r="Q22" s="93">
-        <v>0.41805555555555557</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="R22" s="93">
-        <v>0.4236111111111111</v>
-      </c>
-      <c r="T22" s="93">
         <v>0.43055555555555558</v>
       </c>
-      <c r="U22" s="92">
+      <c r="S22" s="92">
         <v>0.4375</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
@@ -8592,38 +8568,38 @@
       <c r="I23" s="93">
         <v>0.45833333333333331</v>
       </c>
+      <c r="J23" s="93">
+        <v>0.47152777777777777</v>
+      </c>
       <c r="K23" s="93">
-        <v>0.47152777777777777</v>
+        <v>0.47361111111111109</v>
       </c>
       <c r="L23" s="93">
-        <v>0.47361111111111109</v>
+        <v>0.4777777777777778</v>
       </c>
       <c r="M23" s="93">
-        <v>0.4777777777777778</v>
+        <v>0.48125000000000001</v>
       </c>
       <c r="N23" s="93">
-        <v>0.48125000000000001</v>
-      </c>
-      <c r="O23" s="93">
         <v>0.4861111111111111</v>
       </c>
-      <c r="P23" s="92">
+      <c r="O23" s="92">
         <v>0.4909722222222222</v>
       </c>
+      <c r="P23" s="93">
+        <v>0.49652777777777779</v>
+      </c>
       <c r="Q23" s="93">
-        <v>0.49652777777777779</v>
+        <v>0.50138888888888888</v>
       </c>
       <c r="R23" s="93">
-        <v>0.50138888888888888</v>
-      </c>
-      <c r="T23" s="93">
         <v>0.5083333333333333</v>
       </c>
-      <c r="U23" s="93">
+      <c r="S23" s="93">
         <v>0.51388888888888884</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
@@ -8651,38 +8627,38 @@
       <c r="I24" s="93">
         <v>0.41666666666666669</v>
       </c>
+      <c r="J24" s="93">
+        <v>0.43680555555555556</v>
+      </c>
       <c r="K24" s="93">
-        <v>0.43680555555555556</v>
+        <v>0.43888888888888888</v>
       </c>
       <c r="L24" s="93">
-        <v>0.43888888888888888</v>
+        <v>0.44166666666666665</v>
       </c>
       <c r="M24" s="93">
-        <v>0.44166666666666665</v>
+        <v>0.44583333333333336</v>
       </c>
       <c r="N24" s="93">
-        <v>0.44583333333333336</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="O24" s="93">
-        <v>0.4513888888888889</v>
+        <v>0.45694444444444443</v>
       </c>
       <c r="P24" s="93">
-        <v>0.45694444444444443</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="Q24" s="93">
-        <v>0.46250000000000002</v>
+        <v>0.46805555555555556</v>
       </c>
       <c r="R24" s="93">
-        <v>0.46805555555555556</v>
-      </c>
-      <c r="T24" s="93">
         <v>0.48125000000000001</v>
       </c>
-      <c r="U24" s="92">
+      <c r="S24" s="92">
         <v>0.48819444444444443</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
@@ -8710,38 +8686,38 @@
       <c r="I25" s="93">
         <v>0.41666666666666669</v>
       </c>
+      <c r="J25" s="93">
+        <v>0.44374999999999998</v>
+      </c>
       <c r="K25" s="93">
-        <v>0.44374999999999998</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L25" s="93">
-        <v>0.44444444444444442</v>
+        <v>0.44861111111111113</v>
       </c>
       <c r="M25" s="93">
-        <v>0.44861111111111113</v>
+        <v>0.45277777777777778</v>
       </c>
       <c r="N25" s="93">
-        <v>0.45277777777777778</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="O25" s="93">
-        <v>0.45833333333333331</v>
+        <v>0.46319444444444446</v>
       </c>
       <c r="P25" s="93">
-        <v>0.46319444444444446</v>
+        <v>0.46875</v>
       </c>
       <c r="Q25" s="93">
-        <v>0.46875</v>
+        <v>0.47430555555555554</v>
       </c>
       <c r="R25" s="93">
-        <v>0.47430555555555554</v>
-      </c>
-      <c r="T25" s="93">
         <v>0.4826388888888889</v>
       </c>
-      <c r="U25" s="92">
+      <c r="S25" s="92">
         <v>0.49652777777777779</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -8769,38 +8745,38 @@
       <c r="I26" s="93">
         <v>0.5625</v>
       </c>
+      <c r="J26" s="93">
+        <v>0.57847222222222228</v>
+      </c>
       <c r="K26" s="93">
-        <v>0.57847222222222228</v>
+        <v>0.57986111111111116</v>
       </c>
       <c r="L26" s="93">
-        <v>0.57986111111111116</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="M26" s="93">
-        <v>0.58333333333333337</v>
+        <v>0.58750000000000002</v>
       </c>
       <c r="N26" s="93">
-        <v>0.58750000000000002</v>
+        <v>0.59236111111111112</v>
       </c>
       <c r="O26" s="93">
-        <v>0.59236111111111112</v>
+        <v>0.59652777777777777</v>
       </c>
       <c r="P26" s="93">
-        <v>0.59652777777777777</v>
+        <v>0.6020833333333333</v>
       </c>
       <c r="Q26" s="93">
-        <v>0.6020833333333333</v>
+        <v>0.6069444444444444</v>
       </c>
       <c r="R26" s="93">
-        <v>0.6069444444444444</v>
-      </c>
-      <c r="T26" s="93">
         <v>0.61458333333333337</v>
       </c>
-      <c r="U26" s="92">
+      <c r="S26" s="92">
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -8828,38 +8804,38 @@
       <c r="I27" s="93">
         <v>0.58333333333333337</v>
       </c>
+      <c r="J27" s="93">
+        <v>0.6</v>
+      </c>
       <c r="K27" s="93">
-        <v>0.6</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="L27" s="93">
-        <v>0.60069444444444442</v>
+        <v>0.60486111111111107</v>
       </c>
       <c r="M27" s="93">
-        <v>0.60486111111111107</v>
+        <v>0.60902777777777772</v>
       </c>
       <c r="N27" s="93">
-        <v>0.60902777777777772</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="O27" s="93">
-        <v>0.61458333333333337</v>
+        <v>0.62430555555555556</v>
       </c>
       <c r="P27" s="93">
-        <v>0.62430555555555556</v>
+        <v>0.62986111111111109</v>
       </c>
       <c r="Q27" s="93">
-        <v>0.62986111111111109</v>
+        <v>0.63472222222222219</v>
       </c>
       <c r="R27" s="93">
-        <v>0.63472222222222219</v>
-      </c>
-      <c r="T27" s="93">
         <v>0.64097222222222228</v>
       </c>
-      <c r="U27" s="92">
+      <c r="S27" s="92">
         <v>0.64930555555555558</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
@@ -8887,38 +8863,38 @@
       <c r="I28" s="93">
         <v>0.54166666666666663</v>
       </c>
+      <c r="J28" s="93">
+        <v>0.55694444444444446</v>
+      </c>
       <c r="K28" s="93">
-        <v>0.55694444444444446</v>
+        <v>0.55972222222222223</v>
       </c>
       <c r="L28" s="93">
-        <v>0.55972222222222223</v>
+        <v>0.56388888888888888</v>
       </c>
       <c r="M28" s="93">
-        <v>0.56388888888888888</v>
+        <v>0.56736111111111109</v>
       </c>
       <c r="N28" s="93">
-        <v>0.56736111111111109</v>
+        <v>0.57222222222222219</v>
       </c>
       <c r="O28" s="93">
-        <v>0.57222222222222219</v>
+        <v>0.57708333333333328</v>
       </c>
       <c r="P28" s="93">
-        <v>0.57708333333333328</v>
+        <v>0.58194444444444449</v>
       </c>
       <c r="Q28" s="93">
-        <v>0.58194444444444449</v>
+        <v>0.58750000000000002</v>
       </c>
       <c r="R28" s="93">
-        <v>0.58750000000000002</v>
-      </c>
-      <c r="T28" s="93">
         <v>0.59444444444444444</v>
       </c>
-      <c r="U28" s="92">
+      <c r="S28" s="92">
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
@@ -8946,38 +8922,38 @@
       <c r="I29" s="93">
         <v>0.4375</v>
       </c>
+      <c r="J29" s="93">
+        <v>0.45347222222222222</v>
+      </c>
       <c r="K29" s="93">
-        <v>0.45347222222222222</v>
+        <v>0.4548611111111111</v>
       </c>
       <c r="L29" s="93">
-        <v>0.4548611111111111</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="M29" s="93">
-        <v>0.4597222222222222</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="N29" s="93">
-        <v>0.46250000000000002</v>
+        <v>0.46736111111111112</v>
       </c>
       <c r="O29" s="93">
-        <v>0.46736111111111112</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="P29" s="93">
-        <v>0.47222222222222221</v>
+        <v>0.47708333333333336</v>
       </c>
       <c r="Q29" s="93">
-        <v>0.47708333333333336</v>
+        <v>0.48194444444444445</v>
       </c>
       <c r="R29" s="93">
-        <v>0.48194444444444445</v>
-      </c>
-      <c r="T29" s="93">
         <v>0.4909722222222222</v>
       </c>
-      <c r="U29" s="92">
+      <c r="S29" s="92">
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
@@ -9005,38 +8981,38 @@
       <c r="I30" s="93">
         <v>0.66666666666666663</v>
       </c>
+      <c r="J30" s="93">
+        <v>0.68333333333333335</v>
+      </c>
       <c r="K30" s="93">
-        <v>0.68333333333333335</v>
+        <v>0.68472222222222223</v>
       </c>
       <c r="L30" s="93">
-        <v>0.68472222222222223</v>
+        <v>0.6875</v>
       </c>
       <c r="M30" s="93">
-        <v>0.6875</v>
+        <v>0.69305555555555554</v>
       </c>
       <c r="N30" s="93">
-        <v>0.69305555555555554</v>
+        <v>0.69722222222222219</v>
       </c>
       <c r="O30" s="93">
-        <v>0.69722222222222219</v>
+        <v>0.70277777777777772</v>
       </c>
       <c r="P30" s="93">
-        <v>0.70277777777777772</v>
+        <v>0.70763888888888893</v>
       </c>
       <c r="Q30" s="93">
-        <v>0.70763888888888893</v>
+        <v>0.71250000000000002</v>
       </c>
       <c r="R30" s="93">
-        <v>0.71250000000000002</v>
-      </c>
-      <c r="T30" s="93">
         <v>0.71875</v>
       </c>
-      <c r="U30" s="92">
+      <c r="S30" s="92">
         <v>0.73611111111111116</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -9064,38 +9040,38 @@
       <c r="I31" s="93">
         <v>0.5625</v>
       </c>
+      <c r="J31" s="93">
+        <v>0.5756944444444444</v>
+      </c>
       <c r="K31" s="93">
-        <v>0.5756944444444444</v>
+        <v>0.57708333333333328</v>
       </c>
       <c r="L31" s="93">
-        <v>0.57708333333333328</v>
+        <v>0.5805555555555556</v>
       </c>
       <c r="M31" s="93">
-        <v>0.5805555555555556</v>
+        <v>0.58402777777777781</v>
       </c>
       <c r="N31" s="93">
-        <v>0.58402777777777781</v>
+        <v>0.58888888888888891</v>
       </c>
       <c r="O31" s="93">
-        <v>0.58888888888888891</v>
+        <v>0.59375</v>
       </c>
       <c r="P31" s="93">
-        <v>0.59375</v>
+        <v>0.59861111111111109</v>
       </c>
       <c r="Q31" s="93">
-        <v>0.59861111111111109</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="R31" s="93">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="T31" s="93">
         <v>0.61111111111111116</v>
       </c>
-      <c r="U31" s="92">
+      <c r="S31" s="92">
         <v>0.625</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -9123,38 +9099,38 @@
       <c r="I32" s="93">
         <v>0.40625</v>
       </c>
+      <c r="J32" s="93">
+        <v>0.4201388888888889</v>
+      </c>
       <c r="K32" s="93">
-        <v>0.4201388888888889</v>
+        <v>0.42152777777777778</v>
       </c>
       <c r="L32" s="93">
-        <v>0.42152777777777778</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="M32" s="93">
-        <v>0.42569444444444443</v>
+        <v>0.4284722222222222</v>
       </c>
       <c r="N32" s="93">
-        <v>0.4284722222222222</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="O32" s="93">
-        <v>0.43333333333333335</v>
+        <v>0.43888888888888888</v>
       </c>
       <c r="P32" s="93">
-        <v>0.43888888888888888</v>
+        <v>0.44374999999999998</v>
       </c>
       <c r="Q32" s="93">
-        <v>0.44374999999999998</v>
+        <v>0.44861111111111113</v>
       </c>
       <c r="R32" s="93">
-        <v>0.44861111111111113</v>
-      </c>
-      <c r="T32" s="93">
         <v>0.4548611111111111</v>
       </c>
-      <c r="U32" s="92">
+      <c r="S32" s="92">
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -9182,38 +9158,38 @@
       <c r="I33" s="93">
         <v>0.56944444444444442</v>
       </c>
+      <c r="J33" s="93">
+        <v>0.58194444444444449</v>
+      </c>
       <c r="K33" s="93">
-        <v>0.58194444444444449</v>
+        <v>0.58611111111111114</v>
       </c>
       <c r="L33" s="93">
-        <v>0.58611111111111114</v>
+        <v>0.58958333333333335</v>
       </c>
       <c r="M33" s="93">
-        <v>0.58958333333333335</v>
+        <v>0.59444444444444444</v>
       </c>
       <c r="N33" s="93">
-        <v>0.59444444444444444</v>
+        <v>0.59930555555555554</v>
       </c>
       <c r="O33" s="93">
-        <v>0.59930555555555554</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="P33" s="93">
-        <v>0.60416666666666663</v>
+        <v>0.61111111111111116</v>
       </c>
       <c r="Q33" s="93">
-        <v>0.61111111111111116</v>
+        <v>0.62152777777777779</v>
       </c>
       <c r="R33" s="93">
-        <v>0.62152777777777779</v>
-      </c>
-      <c r="T33" s="93">
         <v>0.62777777777777777</v>
       </c>
-      <c r="U33" s="92">
+      <c r="S33" s="92">
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
@@ -9241,38 +9217,38 @@
       <c r="I34" s="93">
         <v>0.34027777777777779</v>
       </c>
+      <c r="J34" s="93">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="K34" s="93">
-        <v>0.35416666666666669</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="L34" s="93">
-        <v>0.35555555555555557</v>
+        <v>0.35902777777777778</v>
       </c>
       <c r="M34" s="93">
-        <v>0.35902777777777778</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="N34" s="93">
-        <v>0.36249999999999999</v>
+        <v>0.36736111111111114</v>
       </c>
       <c r="O34" s="93">
-        <v>0.36736111111111114</v>
+        <v>0.37291666666666667</v>
       </c>
       <c r="P34" s="93">
-        <v>0.37291666666666667</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="Q34" s="93">
-        <v>0.37777777777777777</v>
+        <v>0.38333333333333336</v>
       </c>
       <c r="R34" s="93">
-        <v>0.38333333333333336</v>
-      </c>
-      <c r="T34" s="93">
         <v>0.39097222222222222</v>
       </c>
-      <c r="U34" s="92">
+      <c r="S34" s="92">
         <v>0.39930555555555558</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -9300,38 +9276,38 @@
       <c r="I35" s="93">
         <v>0.5</v>
       </c>
+      <c r="J35" s="93">
+        <v>0.51527777777777772</v>
+      </c>
       <c r="K35" s="93">
-        <v>0.51527777777777772</v>
+        <v>0.51736111111111116</v>
       </c>
       <c r="L35" s="93">
-        <v>0.51736111111111116</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="M35" s="93">
-        <v>0.52083333333333337</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="N35" s="93">
-        <v>0.52500000000000002</v>
+        <v>0.52986111111111112</v>
       </c>
       <c r="O35" s="93">
-        <v>0.52986111111111112</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="P35" s="93">
-        <v>0.53472222222222221</v>
+        <v>0.5395833333333333</v>
       </c>
       <c r="Q35" s="93">
-        <v>0.5395833333333333</v>
+        <v>0.54374999999999996</v>
       </c>
       <c r="R35" s="93">
-        <v>0.54374999999999996</v>
-      </c>
-      <c r="T35" s="93">
         <v>0.55000000000000004</v>
       </c>
-      <c r="U35" s="92">
+      <c r="S35" s="92">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -9359,38 +9335,38 @@
       <c r="I36" s="93">
         <v>0.38194444444444442</v>
       </c>
+      <c r="J36" s="93">
+        <v>0.39652777777777776</v>
+      </c>
       <c r="K36" s="93">
-        <v>0.39652777777777776</v>
+        <v>0.39791666666666664</v>
       </c>
       <c r="L36" s="93">
-        <v>0.39791666666666664</v>
+        <v>0.40138888888888891</v>
       </c>
       <c r="M36" s="93">
-        <v>0.40138888888888891</v>
+        <v>0.40625</v>
       </c>
       <c r="N36" s="93">
-        <v>0.40625</v>
+        <v>0.41041666666666665</v>
       </c>
       <c r="O36" s="93">
-        <v>0.41041666666666665</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="P36" s="93">
-        <v>0.4152777777777778</v>
+        <v>0.42083333333333334</v>
       </c>
       <c r="Q36" s="93">
-        <v>0.42083333333333334</v>
+        <v>0.42569444444444443</v>
       </c>
       <c r="R36" s="93">
-        <v>0.42569444444444443</v>
-      </c>
-      <c r="T36" s="93">
         <v>0.43194444444444446</v>
       </c>
-      <c r="U36" s="92">
+      <c r="S36" s="92">
         <v>0.44097222222222221</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -9418,40 +9394,40 @@
       <c r="I37" s="93">
         <v>0.69444444444444442</v>
       </c>
+      <c r="J37" s="93">
+        <v>0.71527777777777779</v>
+      </c>
       <c r="K37" s="93">
-        <v>0.71527777777777779</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="L37" s="93">
-        <v>0.71666666666666667</v>
+        <v>0.72083333333333333</v>
       </c>
       <c r="M37" s="93">
-        <v>0.72083333333333333</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="N37" s="93">
-        <v>0.72430555555555554</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="O37" s="93">
-        <v>0.72916666666666663</v>
+        <v>0.73472222222222228</v>
       </c>
       <c r="P37" s="93">
-        <v>0.73472222222222228</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="Q37" s="93">
-        <v>0.73958333333333337</v>
+        <v>0.74513888888888891</v>
       </c>
       <c r="R37" s="93">
-        <v>0.74513888888888891</v>
-      </c>
-      <c r="T37" s="93">
         <v>0.75208333333333333</v>
       </c>
-      <c r="U37" s="92">
+      <c r="S37" s="92">
         <v>0.76041666666666663</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U37" xr:uid="{B7A5247D-4E00-4B4A-AEA2-655372E0F049}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U37">
+  <autoFilter ref="A1:S37" xr:uid="{B7A5247D-4E00-4B4A-AEA2-655372E0F049}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S37">
       <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>

</xml_diff>